<commit_message>
Removing phone validation for training, adding some permissions, translations, basic contact summary, add group info to RP flow
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/enroll.xlsx
+++ b/config/itech-aurum/forms/app/enroll.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-59\itech-aurum\forms\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-78\itech-aurum\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A11120-F060-45AC-8BBF-48F9F0F30D3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76132AD0-D3A9-46AA-A362-0CAC7C92A575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="157">
   <si>
     <t>type</t>
   </si>
@@ -213,9 +213,6 @@
   </si>
   <si>
     <t>number</t>
-  </si>
-  <si>
-    <t>Please enter a valid mobile number</t>
   </si>
   <si>
     <t>select_one language_preference</t>
@@ -467,9 +464,6 @@
     <t>This should be in Rands i.e. ZAR</t>
   </si>
   <si>
-    <t>Should start with the country code +27xxxxxxxxx</t>
-  </si>
-  <si>
     <t>weekly</t>
   </si>
   <si>
@@ -497,13 +491,13 @@
     <t>Please confirm consent</t>
   </si>
   <si>
-    <t>regex(., '^\+27[0-9]{9}$')</t>
-  </si>
-  <si>
     <t>selected(../mobile_company, 'other')</t>
   </si>
   <si>
     <t>../person/randomization</t>
+  </si>
+  <si>
+    <t>Temporarily disabled validation for testing</t>
   </si>
 </sst>
 </file>
@@ -1098,10 +1092,10 @@
   <dimension ref="A1:AA1022"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A18" sqref="A18:XFD18"/>
+      <selection pane="bottomRight" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -1144,7 +1138,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H1" s="33" t="s">
         <v>6</v>
@@ -1857,7 +1851,7 @@
         <v>42</v>
       </c>
       <c r="B21" s="76" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" s="50"/>
       <c r="D21" s="64"/>
@@ -1869,7 +1863,7 @@
       <c r="J21" s="50"/>
       <c r="K21" s="16"/>
       <c r="L21" s="64" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
@@ -2216,7 +2210,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D31" s="67"/>
       <c r="E31" s="18"/>
@@ -2228,7 +2222,7 @@
         <v>58</v>
       </c>
       <c r="I31" s="53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J31" s="53"/>
       <c r="K31" s="19"/>
@@ -2257,7 +2251,7 @@
         <v>60</v>
       </c>
       <c r="C32" s="54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D32" s="68"/>
       <c r="E32" s="21" t="s">
@@ -2268,10 +2262,10 @@
       </c>
       <c r="G32" s="71"/>
       <c r="H32" s="36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I32" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J32" s="52"/>
       <c r="K32" s="17"/>
@@ -2297,10 +2291,10 @@
         <v>18</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C33" s="54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D33" s="68"/>
       <c r="E33" s="36" t="s">
@@ -2311,10 +2305,10 @@
       </c>
       <c r="G33" s="54"/>
       <c r="H33" s="36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I33" s="52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J33" s="52"/>
       <c r="K33" s="17"/>
@@ -2337,13 +2331,13 @@
     </row>
     <row r="34" spans="1:27" ht="30.75">
       <c r="A34" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B34" s="37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C34" s="54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D34" s="68"/>
       <c r="E34" s="35"/>
@@ -2372,13 +2366,13 @@
     </row>
     <row r="35" spans="1:27" ht="15.75">
       <c r="A35" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="37" t="s">
+      <c r="C35" s="54" t="s">
         <v>89</v>
-      </c>
-      <c r="C35" s="54" t="s">
-        <v>90</v>
       </c>
       <c r="D35" s="68"/>
       <c r="E35" s="35"/>
@@ -2386,7 +2380,7 @@
         <v>33</v>
       </c>
       <c r="G35" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H35" s="35"/>
       <c r="I35" s="54"/>
@@ -2411,13 +2405,13 @@
     </row>
     <row r="36" spans="1:27" ht="15.75">
       <c r="A36" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="B36" s="37" t="s">
+      <c r="C36" s="54" t="s">
         <v>92</v>
-      </c>
-      <c r="C36" s="54" t="s">
-        <v>93</v>
       </c>
       <c r="D36" s="68"/>
       <c r="E36" s="35"/>
@@ -2454,7 +2448,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D37" s="68"/>
       <c r="E37" s="35" t="s">
@@ -2464,14 +2458,10 @@
         <v>33</v>
       </c>
       <c r="G37" s="54"/>
-      <c r="H37" s="35" t="s">
+      <c r="H37" s="35"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="54" t="s">
         <v>156</v>
-      </c>
-      <c r="I37" s="54" t="s">
-        <v>62</v>
-      </c>
-      <c r="J37" s="54" t="s">
-        <v>146</v>
       </c>
       <c r="K37" s="35"/>
       <c r="L37" s="68"/>
@@ -2493,13 +2483,13 @@
     </row>
     <row r="38" spans="1:27" ht="30.75">
       <c r="A38" s="37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B38" s="37" t="s">
         <v>51</v>
       </c>
       <c r="C38" s="54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D38" s="68"/>
       <c r="E38" s="35"/>
@@ -2530,13 +2520,13 @@
     </row>
     <row r="39" spans="1:27" ht="15.75">
       <c r="A39" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="B39" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="37" t="s">
+      <c r="C39" s="54" t="s">
         <v>96</v>
-      </c>
-      <c r="C39" s="54" t="s">
-        <v>97</v>
       </c>
       <c r="D39" s="68"/>
       <c r="E39" s="35"/>
@@ -2570,13 +2560,13 @@
         <v>18</v>
       </c>
       <c r="B40" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="C40" s="54" t="s">
         <v>142</v>
       </c>
-      <c r="C40" s="54" t="s">
-        <v>143</v>
-      </c>
       <c r="D40" s="68" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E40" s="35"/>
       <c r="F40" s="35" t="s">
@@ -2606,13 +2596,13 @@
     </row>
     <row r="41" spans="1:27" ht="30.75">
       <c r="A41" s="37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C41" s="54" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D41" s="68"/>
       <c r="E41" s="35"/>
@@ -2621,13 +2611,13 @@
       </c>
       <c r="G41" s="54"/>
       <c r="H41" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="I41" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="I41" s="54" t="s">
-        <v>100</v>
-      </c>
       <c r="J41" s="54" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K41" s="35"/>
       <c r="L41" s="68"/>
@@ -2679,10 +2669,10 @@
         <v>13</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C43" s="56" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D43" s="70"/>
       <c r="E43" s="37" t="s">
@@ -2713,23 +2703,23 @@
     </row>
     <row r="44" spans="1:27" ht="30.75">
       <c r="A44" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="B44" s="37" t="s">
+      <c r="C44" s="54" t="s">
         <v>103</v>
-      </c>
-      <c r="C44" s="54" t="s">
-        <v>104</v>
       </c>
       <c r="D44" s="68"/>
       <c r="E44" s="35"/>
       <c r="F44" s="35"/>
       <c r="G44" s="54"/>
       <c r="H44" s="35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I44" s="54" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J44" s="54"/>
       <c r="K44" s="35"/>
@@ -2752,23 +2742,23 @@
     </row>
     <row r="45" spans="1:27" ht="15.75">
       <c r="A45" s="37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C45" s="54" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D45" s="68"/>
       <c r="E45" s="35"/>
       <c r="F45" s="35"/>
       <c r="G45" s="54"/>
       <c r="H45" s="35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I45" s="54" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J45" s="54"/>
       <c r="K45" s="35"/>
@@ -2849,13 +2839,13 @@
     </row>
     <row r="48" spans="1:27" ht="30.75">
       <c r="A48" s="37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C48" s="54" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D48" s="68"/>
       <c r="E48" s="35"/>
@@ -2864,10 +2854,10 @@
       </c>
       <c r="G48" s="54"/>
       <c r="H48" s="35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I48" s="54" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J48" s="54"/>
       <c r="K48" s="54"/>
@@ -2890,13 +2880,13 @@
     </row>
     <row r="49" spans="1:27" ht="15.75">
       <c r="A49" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="B49" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="B49" s="37" t="s">
+      <c r="C49" s="54" t="s">
         <v>111</v>
-      </c>
-      <c r="C49" s="54" t="s">
-        <v>112</v>
       </c>
       <c r="D49" s="68"/>
       <c r="E49" s="35"/>
@@ -2904,7 +2894,7 @@
         <v>33</v>
       </c>
       <c r="G49" s="54" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H49" s="35"/>
       <c r="I49" s="54"/>
@@ -2929,16 +2919,16 @@
     </row>
     <row r="50" spans="1:27" ht="26.25">
       <c r="A50" s="37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C50" s="54" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D50" s="68" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E50" s="35"/>
       <c r="F50" s="35" t="s">
@@ -2946,10 +2936,10 @@
       </c>
       <c r="G50" s="54"/>
       <c r="H50" s="35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I50" s="54" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J50" s="54"/>
       <c r="K50" s="54"/>
@@ -30931,7 +30921,7 @@
   <sheetData>
     <row r="1" spans="1:26" s="32" customFormat="1" ht="15.75">
       <c r="A1" s="41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="41" t="s">
         <v>1</v>
@@ -30965,13 +30955,13 @@
     </row>
     <row r="2" spans="1:26" ht="15.75">
       <c r="A2" s="39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -30999,13 +30989,13 @@
     </row>
     <row r="3" spans="1:26" ht="15.75">
       <c r="A3" s="39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -31064,10 +31054,10 @@
         <v>51</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -31098,10 +31088,10 @@
         <v>51</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -31132,10 +31122,10 @@
         <v>51</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -31191,13 +31181,13 @@
     </row>
     <row r="9" spans="1:26" ht="15.75">
       <c r="A9" s="39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -31225,13 +31215,13 @@
     </row>
     <row r="10" spans="1:26" ht="15.75">
       <c r="A10" s="39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -31259,13 +31249,13 @@
     </row>
     <row r="11" spans="1:26" ht="15.75">
       <c r="A11" s="39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -31293,13 +31283,13 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
       <c r="A12" s="39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -31355,13 +31345,13 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
       <c r="A14" s="39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B14" s="39" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -31389,13 +31379,13 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
       <c r="A15" s="39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B15" s="39" t="s">
         <v>59</v>
       </c>
       <c r="C15" s="39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -31451,13 +31441,13 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1">
       <c r="A17" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B17" s="39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -31485,13 +31475,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1">
       <c r="A18" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -31519,13 +31509,13 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1">
       <c r="A19" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C19" s="39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -31553,13 +31543,13 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1">
       <c r="A20" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B20" s="43" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -31587,13 +31577,13 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" s="43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -58803,19 +58793,19 @@
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1">
       <c r="A1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>73</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -58830,19 +58820,19 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" s="12">
         <v>43900</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>

</xml_diff>

<commit_message>
Adding mute and unmute forms, "patient" role in enroll form, translations
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/enroll.xlsx
+++ b/config/itech-aurum/forms/app/enroll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-78\itech-aurum\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76132AD0-D3A9-46AA-A362-0CAC7C92A575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDF50AF-D0A0-416D-9BDF-86103402D8DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="159">
   <si>
     <t>type</t>
   </si>
@@ -498,6 +498,12 @@
   </si>
   <si>
     <t>Temporarily disabled validation for testing</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>"patient"</t>
   </si>
 </sst>
 </file>
@@ -1089,13 +1095,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA1022"/>
+  <dimension ref="A1:AA1023"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I37" sqref="I37"/>
+      <selection pane="bottomRight" activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -2178,9 +2184,7 @@
       <c r="F30" s="17"/>
       <c r="G30" s="52"/>
       <c r="H30" s="17"/>
-      <c r="I30" s="52" t="s">
-        <v>46</v>
-      </c>
+      <c r="I30" s="52"/>
       <c r="J30" s="52"/>
       <c r="K30" s="17"/>
       <c r="L30" s="66" t="s">
@@ -2202,113 +2206,105 @@
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
     </row>
-    <row r="31" spans="1:27" ht="30.75">
-      <c r="A31" s="24" t="s">
+    <row r="31" spans="1:27" ht="15.75">
+      <c r="A31" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" s="52"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="66" t="s">
+        <v>158</v>
+      </c>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="1"/>
+    </row>
+    <row r="32" spans="1:27" ht="30.75">
+      <c r="A32" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B32" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C32" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="67"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18" t="s">
+      <c r="D32" s="67"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G31" s="53"/>
-      <c r="H31" s="18" t="s">
+      <c r="G32" s="53"/>
+      <c r="H32" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="I31" s="53" t="s">
+      <c r="I32" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="J31" s="53"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="67"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
-      <c r="S31" s="3"/>
-      <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
-      <c r="V31" s="3"/>
-      <c r="W31" s="3"/>
-      <c r="X31" s="3"/>
-      <c r="Y31" s="3"/>
-      <c r="Z31" s="3"/>
-      <c r="AA31" s="3"/>
-    </row>
-    <row r="32" spans="1:27" ht="30.75">
-      <c r="A32" s="25" t="s">
+      <c r="J32" s="53"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="67"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AA32" s="3"/>
+    </row>
+    <row r="33" spans="1:27" ht="30.75">
+      <c r="A33" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B33" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="54" t="s">
+      <c r="C33" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="68"/>
-      <c r="E32" s="21" t="s">
+      <c r="D33" s="68"/>
+      <c r="E33" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="F33" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="71"/>
-      <c r="H32" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="I32" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="J32" s="52"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="68"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="1"/>
-      <c r="T32" s="1"/>
-      <c r="U32" s="1"/>
-      <c r="V32" s="1"/>
-      <c r="W32" s="1"/>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
-      <c r="Z32" s="1"/>
-      <c r="AA32" s="1"/>
-    </row>
-    <row r="33" spans="1:27" ht="30.75">
-      <c r="A33" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="54" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="68"/>
-      <c r="E33" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="F33" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G33" s="54"/>
+      <c r="G33" s="71"/>
       <c r="H33" s="36" t="s">
         <v>79</v>
       </c>
       <c r="I33" s="52" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J33" s="52"/>
       <c r="K33" s="17"/>
@@ -2331,57 +2327,61 @@
     </row>
     <row r="34" spans="1:27" ht="30.75">
       <c r="A34" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="68"/>
+      <c r="E34" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G34" s="54"/>
+      <c r="H34" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="I34" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="J34" s="52"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="68"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
+      <c r="Z34" s="1"/>
+      <c r="AA34" s="1"/>
+    </row>
+    <row r="35" spans="1:27" ht="30.75">
+      <c r="A35" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="37" t="s">
+      <c r="B35" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="C34" s="54" t="s">
+      <c r="C35" s="54" t="s">
         <v>86</v>
-      </c>
-      <c r="D34" s="68"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="54"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="54"/>
-      <c r="J34" s="54"/>
-      <c r="K34" s="35"/>
-      <c r="L34" s="68"/>
-      <c r="M34" s="35"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
-      <c r="R34" s="3"/>
-      <c r="S34" s="3"/>
-      <c r="T34" s="3"/>
-      <c r="U34" s="3"/>
-      <c r="V34" s="3"/>
-      <c r="W34" s="3"/>
-      <c r="X34" s="3"/>
-      <c r="Y34" s="3"/>
-      <c r="Z34" s="1"/>
-      <c r="AA34" s="1"/>
-    </row>
-    <row r="35" spans="1:27" ht="15.75">
-      <c r="A35" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="B35" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="C35" s="54" t="s">
-        <v>89</v>
       </c>
       <c r="D35" s="68"/>
       <c r="E35" s="35"/>
-      <c r="F35" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G35" s="54" t="s">
-        <v>153</v>
-      </c>
+      <c r="F35" s="35"/>
+      <c r="G35" s="54"/>
       <c r="H35" s="35"/>
       <c r="I35" s="54"/>
       <c r="J35" s="54"/>
@@ -2405,64 +2405,62 @@
     </row>
     <row r="36" spans="1:27" ht="15.75">
       <c r="A36" s="37" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C36" s="54" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D36" s="68"/>
       <c r="E36" s="35"/>
       <c r="F36" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="G36" s="54"/>
+      <c r="G36" s="54" t="s">
+        <v>153</v>
+      </c>
       <c r="H36" s="35"/>
       <c r="I36" s="54"/>
       <c r="J36" s="54"/>
       <c r="K36" s="35"/>
       <c r="L36" s="68"/>
       <c r="M36" s="35"/>
-      <c r="N36" s="20"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
-      <c r="R36" s="1"/>
-      <c r="S36" s="1"/>
-      <c r="T36" s="1"/>
-      <c r="U36" s="1"/>
-      <c r="V36" s="1"/>
-      <c r="W36" s="1"/>
-      <c r="X36" s="4"/>
-      <c r="Y36" s="4"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="3"/>
+      <c r="X36" s="3"/>
+      <c r="Y36" s="3"/>
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
     </row>
-    <row r="37" spans="1:27" ht="30.75">
+    <row r="37" spans="1:27" ht="15.75">
       <c r="A37" s="37" t="s">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="C37" s="54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D37" s="68"/>
-      <c r="E37" s="35" t="s">
-        <v>61</v>
-      </c>
+      <c r="E37" s="35"/>
       <c r="F37" s="35" t="s">
         <v>33</v>
       </c>
       <c r="G37" s="54"/>
       <c r="H37" s="35"/>
       <c r="I37" s="54"/>
-      <c r="J37" s="54" t="s">
-        <v>156</v>
-      </c>
+      <c r="J37" s="54"/>
       <c r="K37" s="35"/>
       <c r="L37" s="68"/>
       <c r="M37" s="35"/>
@@ -2483,50 +2481,54 @@
     </row>
     <row r="38" spans="1:27" ht="30.75">
       <c r="A38" s="37" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C38" s="54" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="D38" s="68"/>
-      <c r="E38" s="35"/>
+      <c r="E38" s="35" t="s">
+        <v>61</v>
+      </c>
       <c r="F38" s="35" t="s">
         <v>33</v>
       </c>
       <c r="G38" s="54"/>
       <c r="H38" s="35"/>
       <c r="I38" s="54"/>
-      <c r="J38" s="54"/>
+      <c r="J38" s="54" t="s">
+        <v>156</v>
+      </c>
       <c r="K38" s="35"/>
       <c r="L38" s="68"/>
       <c r="M38" s="35"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="2"/>
-      <c r="R38" s="2"/>
-      <c r="S38" s="2"/>
-      <c r="T38" s="2"/>
-      <c r="U38" s="2"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
-      <c r="X38" s="1"/>
-      <c r="Y38" s="1"/>
+      <c r="X38" s="4"/>
+      <c r="Y38" s="4"/>
       <c r="Z38" s="1"/>
       <c r="AA38" s="1"/>
     </row>
-    <row r="39" spans="1:27" ht="15.75">
+    <row r="39" spans="1:27" ht="30.75">
       <c r="A39" s="37" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="C39" s="54" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="D39" s="68"/>
       <c r="E39" s="35"/>
@@ -2540,37 +2542,35 @@
       <c r="K39" s="35"/>
       <c r="L39" s="68"/>
       <c r="M39" s="35"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-      <c r="V39" s="3"/>
-      <c r="W39" s="3"/>
-      <c r="X39" s="3"/>
-      <c r="Y39" s="3"/>
-      <c r="Z39" s="3"/>
-      <c r="AA39" s="3"/>
-    </row>
-    <row r="40" spans="1:27" ht="26.25">
+      <c r="N39" s="17"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+      <c r="Y39" s="1"/>
+      <c r="Z39" s="1"/>
+      <c r="AA39" s="1"/>
+    </row>
+    <row r="40" spans="1:27" ht="15.75">
       <c r="A40" s="37" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="C40" s="54" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
-      <c r="D40" s="68" t="s">
-        <v>154</v>
-      </c>
+      <c r="D40" s="68"/>
       <c r="E40" s="35"/>
       <c r="F40" s="35" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="G40" s="54"/>
       <c r="H40" s="35"/>
@@ -2580,113 +2580,115 @@
       <c r="L40" s="68"/>
       <c r="M40" s="35"/>
       <c r="N40" s="18"/>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5"/>
-      <c r="Q40" s="5"/>
-      <c r="R40" s="5"/>
-      <c r="S40" s="5"/>
-      <c r="T40" s="5"/>
-      <c r="U40" s="5"/>
-      <c r="V40" s="5"/>
-      <c r="W40" s="5"/>
-      <c r="X40" s="5"/>
-      <c r="Y40" s="5"/>
-      <c r="Z40" s="5"/>
-      <c r="AA40" s="5"/>
-    </row>
-    <row r="41" spans="1:27" ht="30.75">
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3"/>
+      <c r="T40" s="3"/>
+      <c r="U40" s="3"/>
+      <c r="V40" s="3"/>
+      <c r="W40" s="3"/>
+      <c r="X40" s="3"/>
+      <c r="Y40" s="3"/>
+      <c r="Z40" s="3"/>
+      <c r="AA40" s="3"/>
+    </row>
+    <row r="41" spans="1:27" ht="26.25">
       <c r="A41" s="37" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>97</v>
+        <v>141</v>
       </c>
       <c r="C41" s="54" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
-      <c r="D41" s="68"/>
+      <c r="D41" s="68" t="s">
+        <v>154</v>
+      </c>
       <c r="E41" s="35"/>
       <c r="F41" s="35" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="G41" s="54"/>
-      <c r="H41" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="I41" s="54" t="s">
-        <v>99</v>
-      </c>
-      <c r="J41" s="54" t="s">
-        <v>144</v>
-      </c>
+      <c r="H41" s="35"/>
+      <c r="I41" s="54"/>
+      <c r="J41" s="54"/>
       <c r="K41" s="35"/>
       <c r="L41" s="68"/>
       <c r="M41" s="35"/>
       <c r="N41" s="18"/>
-      <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
-      <c r="T41" s="3"/>
-      <c r="U41" s="3"/>
-      <c r="V41" s="3"/>
-      <c r="W41" s="3"/>
-      <c r="X41" s="3"/>
-      <c r="Y41" s="3"/>
-      <c r="Z41" s="3"/>
-      <c r="AA41" s="3"/>
-    </row>
-    <row r="42" spans="1:27" ht="15.75">
-      <c r="A42" s="38"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="58"/>
-      <c r="D42" s="69"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="55"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="55"/>
-      <c r="L42" s="69"/>
-      <c r="M42" s="38"/>
-      <c r="N42" s="38"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-      <c r="Q42" s="2"/>
-      <c r="R42" s="2"/>
-      <c r="S42" s="2"/>
-      <c r="T42" s="2"/>
-      <c r="U42" s="2"/>
-      <c r="V42" s="1"/>
-      <c r="W42" s="1"/>
-      <c r="X42" s="1"/>
-      <c r="Y42" s="1"/>
-      <c r="Z42" s="1"/>
-      <c r="AA42" s="1"/>
-    </row>
-    <row r="43" spans="1:27" ht="15" customHeight="1">
-      <c r="A43" s="37" t="s">
-        <v>13</v>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5"/>
+      <c r="S41" s="5"/>
+      <c r="T41" s="5"/>
+      <c r="U41" s="5"/>
+      <c r="V41" s="5"/>
+      <c r="W41" s="5"/>
+      <c r="X41" s="5"/>
+      <c r="Y41" s="5"/>
+      <c r="Z41" s="5"/>
+      <c r="AA41" s="5"/>
+    </row>
+    <row r="42" spans="1:27" ht="30.75">
+      <c r="A42" s="37" t="s">
+        <v>101</v>
       </c>
-      <c r="B43" s="37" t="s">
-        <v>100</v>
+      <c r="B42" s="37" t="s">
+        <v>97</v>
       </c>
-      <c r="C43" s="56" t="s">
-        <v>152</v>
+      <c r="C42" s="54" t="s">
+        <v>143</v>
       </c>
-      <c r="D43" s="70"/>
-      <c r="E43" s="37" t="s">
-        <v>17</v>
+      <c r="D42" s="68"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35" t="s">
+        <v>33</v>
       </c>
-      <c r="F43" s="37"/>
-      <c r="G43" s="56"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="56"/>
-      <c r="J43" s="56"/>
-      <c r="K43" s="37"/>
-      <c r="L43" s="70"/>
-      <c r="M43" s="37"/>
-      <c r="N43" s="37"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="I42" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="J42" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="K42" s="35"/>
+      <c r="L42" s="68"/>
+      <c r="M42" s="35"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="U42" s="3"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="3"/>
+      <c r="X42" s="3"/>
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="3"/>
+      <c r="AA42" s="3"/>
+    </row>
+    <row r="43" spans="1:27" ht="15.75">
+      <c r="A43" s="38"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="69"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="55"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="55"/>
+      <c r="L43" s="69"/>
+      <c r="M43" s="38"/>
+      <c r="N43" s="38"/>
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
@@ -2694,38 +2696,36 @@
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
-      <c r="V43" s="2"/>
-      <c r="W43" s="2"/>
-      <c r="X43" s="2"/>
-      <c r="Y43" s="2"/>
-      <c r="Z43" s="2"/>
-      <c r="AA43" s="2"/>
-    </row>
-    <row r="44" spans="1:27" ht="30.75">
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
+      <c r="X43" s="1"/>
+      <c r="Y43" s="1"/>
+      <c r="Z43" s="1"/>
+      <c r="AA43" s="1"/>
+    </row>
+    <row r="44" spans="1:27" ht="15" customHeight="1">
       <c r="A44" s="37" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="B44" s="37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
-      <c r="C44" s="54" t="s">
-        <v>103</v>
+      <c r="C44" s="56" t="s">
+        <v>152</v>
       </c>
-      <c r="D44" s="68"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="35" t="s">
-        <v>98</v>
+      <c r="D44" s="70"/>
+      <c r="E44" s="37" t="s">
+        <v>17</v>
       </c>
-      <c r="I44" s="54" t="s">
-        <v>99</v>
-      </c>
-      <c r="J44" s="54"/>
-      <c r="K44" s="35"/>
-      <c r="L44" s="68"/>
-      <c r="M44" s="35"/>
-      <c r="N44" s="35"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="56"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="56"/>
+      <c r="J44" s="56"/>
+      <c r="K44" s="37"/>
+      <c r="L44" s="70"/>
+      <c r="M44" s="37"/>
+      <c r="N44" s="37"/>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
@@ -2740,25 +2740,25 @@
       <c r="Z44" s="2"/>
       <c r="AA44" s="2"/>
     </row>
-    <row r="45" spans="1:27" ht="15.75">
+    <row r="45" spans="1:27" ht="30.75">
       <c r="A45" s="37" t="s">
         <v>101</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C45" s="54" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D45" s="68"/>
       <c r="E45" s="35"/>
       <c r="F45" s="35"/>
       <c r="G45" s="54"/>
       <c r="H45" s="35" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="I45" s="54" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="J45" s="54"/>
       <c r="K45" s="35"/>
@@ -2779,23 +2779,31 @@
       <c r="Z45" s="2"/>
       <c r="AA45" s="2"/>
     </row>
-    <row r="46" spans="1:27" ht="12.75" customHeight="1">
+    <row r="46" spans="1:27" ht="15.75">
       <c r="A46" s="37" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
-      <c r="B46" s="37"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="70"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="56"/>
-      <c r="H46" s="37"/>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
-      <c r="K46" s="37"/>
-      <c r="L46" s="70"/>
-      <c r="M46" s="37"/>
-      <c r="N46" s="37"/>
+      <c r="B46" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="D46" s="68"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="54"/>
+      <c r="H46" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="I46" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="J46" s="54"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="68"/>
+      <c r="M46" s="35"/>
+      <c r="N46" s="35"/>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
@@ -2811,18 +2819,22 @@
       <c r="AA46" s="2"/>
     </row>
     <row r="47" spans="1:27" ht="12.75" customHeight="1">
-      <c r="A47" s="38"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="69"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="55"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="55"/>
-      <c r="L47" s="69"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
+      <c r="A47" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="37"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="70"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="56"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="56"/>
+      <c r="J47" s="56"/>
+      <c r="K47" s="37"/>
+      <c r="L47" s="70"/>
+      <c r="M47" s="37"/>
+      <c r="N47" s="37"/>
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
@@ -2837,33 +2849,19 @@
       <c r="Z47" s="2"/>
       <c r="AA47" s="2"/>
     </row>
-    <row r="48" spans="1:27" ht="30.75">
-      <c r="A48" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="B48" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="C48" s="54" t="s">
-        <v>148</v>
-      </c>
-      <c r="D48" s="68"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G48" s="54"/>
-      <c r="H48" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="I48" s="54" t="s">
-        <v>149</v>
-      </c>
-      <c r="J48" s="54"/>
-      <c r="K48" s="54"/>
-      <c r="L48" s="68"/>
-      <c r="M48" s="54"/>
-      <c r="N48" s="54"/>
+    <row r="48" spans="1:27" ht="12.75" customHeight="1">
+      <c r="A48" s="38"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="55"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="38"/>
+      <c r="G48" s="55"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="55"/>
+      <c r="L48" s="69"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
@@ -2878,26 +2876,28 @@
       <c r="Z48" s="2"/>
       <c r="AA48" s="2"/>
     </row>
-    <row r="49" spans="1:27" ht="15.75">
+    <row r="49" spans="1:27" ht="30.75">
       <c r="A49" s="37" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C49" s="54" t="s">
-        <v>111</v>
+        <v>148</v>
       </c>
       <c r="D49" s="68"/>
       <c r="E49" s="35"/>
       <c r="F49" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="G49" s="54" t="s">
-        <v>151</v>
+      <c r="G49" s="54"/>
+      <c r="H49" s="35" t="s">
+        <v>98</v>
       </c>
-      <c r="H49" s="35"/>
-      <c r="I49" s="54"/>
+      <c r="I49" s="54" t="s">
+        <v>149</v>
+      </c>
       <c r="J49" s="54"/>
       <c r="K49" s="54"/>
       <c r="L49" s="68"/>
@@ -2917,30 +2917,26 @@
       <c r="Z49" s="2"/>
       <c r="AA49" s="2"/>
     </row>
-    <row r="50" spans="1:27" ht="26.25">
+    <row r="50" spans="1:27" ht="15.75">
       <c r="A50" s="37" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C50" s="54" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
-      <c r="D50" s="68" t="s">
-        <v>113</v>
-      </c>
+      <c r="D50" s="68"/>
       <c r="E50" s="35"/>
       <c r="F50" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="G50" s="54"/>
-      <c r="H50" s="35" t="s">
-        <v>98</v>
+      <c r="G50" s="54" t="s">
+        <v>151</v>
       </c>
-      <c r="I50" s="54" t="s">
-        <v>149</v>
-      </c>
+      <c r="H50" s="35"/>
+      <c r="I50" s="54"/>
       <c r="J50" s="54"/>
       <c r="K50" s="54"/>
       <c r="L50" s="68"/>
@@ -2960,23 +2956,35 @@
       <c r="Z50" s="2"/>
       <c r="AA50" s="2"/>
     </row>
-    <row r="51" spans="1:27" ht="12.75" customHeight="1">
+    <row r="51" spans="1:27" ht="26.25">
       <c r="A51" s="37" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
-      <c r="B51" s="37"/>
-      <c r="C51" s="56"/>
-      <c r="D51" s="59"/>
-      <c r="E51" s="37"/>
-      <c r="F51" s="37"/>
-      <c r="G51" s="56"/>
-      <c r="H51" s="37"/>
-      <c r="I51" s="56"/>
-      <c r="J51" s="56"/>
-      <c r="K51" s="37"/>
-      <c r="L51" s="70"/>
-      <c r="M51" s="37"/>
-      <c r="N51" s="37"/>
+      <c r="B51" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="D51" s="68" t="s">
+        <v>113</v>
+      </c>
+      <c r="E51" s="35"/>
+      <c r="F51" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G51" s="54"/>
+      <c r="H51" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="I51" s="54" t="s">
+        <v>149</v>
+      </c>
+      <c r="J51" s="54"/>
+      <c r="K51" s="54"/>
+      <c r="L51" s="68"/>
+      <c r="M51" s="54"/>
+      <c r="N51" s="54"/>
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
@@ -2992,20 +3000,22 @@
       <c r="AA51" s="2"/>
     </row>
     <row r="52" spans="1:27" ht="12.75" customHeight="1">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="49"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="49"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="49"/>
-      <c r="J52" s="49"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="49"/>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
+      <c r="A52" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="37"/>
+      <c r="C52" s="56"/>
+      <c r="D52" s="59"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="56"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="56"/>
+      <c r="J52" s="56"/>
+      <c r="K52" s="37"/>
+      <c r="L52" s="70"/>
+      <c r="M52" s="37"/>
+      <c r="N52" s="37"/>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
@@ -8182,7 +8192,7 @@
       <c r="Z230" s="2"/>
       <c r="AA230" s="2"/>
     </row>
-    <row r="231" spans="1:27" ht="15.75" customHeight="1">
+    <row r="231" spans="1:27" ht="12.75" customHeight="1">
       <c r="A231" s="2"/>
       <c r="B231" s="2"/>
       <c r="C231" s="49"/>
@@ -30657,7 +30667,7 @@
       <c r="Z1005" s="2"/>
       <c r="AA1005" s="2"/>
     </row>
-    <row r="1006" spans="1:27" ht="15" customHeight="1">
+    <row r="1006" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1006" s="2"/>
       <c r="B1006" s="2"/>
       <c r="C1006" s="49"/>
@@ -30670,6 +30680,21 @@
       <c r="J1006" s="49"/>
       <c r="K1006" s="2"/>
       <c r="L1006" s="49"/>
+      <c r="M1006" s="2"/>
+      <c r="N1006" s="2"/>
+      <c r="O1006" s="2"/>
+      <c r="P1006" s="2"/>
+      <c r="Q1006" s="2"/>
+      <c r="R1006" s="2"/>
+      <c r="S1006" s="2"/>
+      <c r="T1006" s="2"/>
+      <c r="U1006" s="2"/>
+      <c r="V1006" s="2"/>
+      <c r="W1006" s="2"/>
+      <c r="X1006" s="2"/>
+      <c r="Y1006" s="2"/>
+      <c r="Z1006" s="2"/>
+      <c r="AA1006" s="2"/>
     </row>
     <row r="1007" spans="1:27" ht="15" customHeight="1">
       <c r="A1007" s="2"/>
@@ -30894,6 +30919,20 @@
       <c r="J1022" s="49"/>
       <c r="K1022" s="2"/>
       <c r="L1022" s="49"/>
+    </row>
+    <row r="1023" spans="1:12" ht="15" customHeight="1">
+      <c r="A1023" s="2"/>
+      <c r="B1023" s="2"/>
+      <c r="C1023" s="49"/>
+      <c r="D1023" s="2"/>
+      <c r="E1023" s="2"/>
+      <c r="F1023" s="2"/>
+      <c r="G1023" s="49"/>
+      <c r="H1023" s="2"/>
+      <c r="I1023" s="49"/>
+      <c r="J1023" s="49"/>
+      <c r="K1023" s="2"/>
+      <c r="L1023" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>

</xml_diff>

<commit_message>
Reverting "off" and "on" forms, "mute" and "unmute" remain. Checkbox added for testing/training which disables phone number validation (and temporary test changes to work with this change). #78
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/enroll.xlsx
+++ b/config/itech-aurum/forms/app/enroll.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-78\itech-aurum\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDF50AF-D0A0-416D-9BDF-86103402D8DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04B2CA8-627F-45E9-BED8-D804D6217EC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="164">
   <si>
     <t>type</t>
   </si>
@@ -497,13 +497,28 @@
     <t>../person/randomization</t>
   </si>
   <si>
-    <t>Temporarily disabled validation for testing</t>
-  </si>
-  <si>
     <t>role</t>
   </si>
   <si>
     <t>"patient"</t>
+  </si>
+  <si>
+    <t>Please enter a valid mobile number</t>
+  </si>
+  <si>
+    <t>Should start with the country code +27xxxxxxxxx</t>
+  </si>
+  <si>
+    <t>confirm</t>
+  </si>
+  <si>
+    <t>If you need to test by entering a non-RSA number, check this and you will be able to enter any phone number (no check)</t>
+  </si>
+  <si>
+    <t>regex(., '^\+27[0-9]{9}$') or selected(${confirm}, 'yes')</t>
+  </si>
+  <si>
+    <t>select_multiple yes</t>
   </si>
 </sst>
 </file>
@@ -1095,13 +1110,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA1023"/>
+  <dimension ref="A1:AA1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H21" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L22" sqref="L22"/>
+      <selection pane="bottomRight" activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -2211,7 +2226,7 @@
         <v>42</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C31" s="52"/>
       <c r="D31" s="66"/>
@@ -2223,7 +2238,7 @@
       <c r="J31" s="52"/>
       <c r="K31" s="17"/>
       <c r="L31" s="66" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M31" s="17"/>
       <c r="N31" s="17"/>
@@ -2497,10 +2512,14 @@
         <v>33</v>
       </c>
       <c r="G38" s="54"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="54"/>
+      <c r="H38" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="I38" s="54" t="s">
+        <v>158</v>
+      </c>
       <c r="J38" s="54" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="K38" s="35"/>
       <c r="L38" s="68"/>
@@ -2520,21 +2539,19 @@
       <c r="Z38" s="1"/>
       <c r="AA38" s="1"/>
     </row>
-    <row r="39" spans="1:27" ht="30.75">
+    <row r="39" spans="1:27" ht="15.75">
       <c r="A39" s="37" t="s">
-        <v>62</v>
+        <v>163</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>51</v>
+        <v>160</v>
       </c>
       <c r="C39" s="54" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="D39" s="68"/>
       <c r="E39" s="35"/>
-      <c r="F39" s="35" t="s">
-        <v>33</v>
-      </c>
+      <c r="F39" s="35"/>
       <c r="G39" s="54"/>
       <c r="H39" s="35"/>
       <c r="I39" s="54"/>
@@ -2542,30 +2559,30 @@
       <c r="K39" s="35"/>
       <c r="L39" s="68"/>
       <c r="M39" s="35"/>
-      <c r="N39" s="17"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="2"/>
-      <c r="U39" s="2"/>
+      <c r="N39" s="20"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
-      <c r="X39" s="1"/>
-      <c r="Y39" s="1"/>
+      <c r="X39" s="4"/>
+      <c r="Y39" s="4"/>
       <c r="Z39" s="1"/>
       <c r="AA39" s="1"/>
     </row>
-    <row r="40" spans="1:27" ht="15.75">
+    <row r="40" spans="1:27" ht="30.75">
       <c r="A40" s="37" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="C40" s="54" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="D40" s="68"/>
       <c r="E40" s="35"/>
@@ -2579,37 +2596,35 @@
       <c r="K40" s="35"/>
       <c r="L40" s="68"/>
       <c r="M40" s="35"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
-      <c r="R40" s="3"/>
-      <c r="S40" s="3"/>
-      <c r="T40" s="3"/>
-      <c r="U40" s="3"/>
-      <c r="V40" s="3"/>
-      <c r="W40" s="3"/>
-      <c r="X40" s="3"/>
-      <c r="Y40" s="3"/>
-      <c r="Z40" s="3"/>
-      <c r="AA40" s="3"/>
-    </row>
-    <row r="41" spans="1:27" ht="26.25">
+      <c r="N40" s="17"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
+      <c r="X40" s="1"/>
+      <c r="Y40" s="1"/>
+      <c r="Z40" s="1"/>
+      <c r="AA40" s="1"/>
+    </row>
+    <row r="41" spans="1:27" ht="15.75">
       <c r="A41" s="37" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="C41" s="54" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
-      <c r="D41" s="68" t="s">
-        <v>154</v>
-      </c>
+      <c r="D41" s="68"/>
       <c r="E41" s="35"/>
       <c r="F41" s="35" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="G41" s="54"/>
       <c r="H41" s="35"/>
@@ -2619,113 +2634,115 @@
       <c r="L41" s="68"/>
       <c r="M41" s="35"/>
       <c r="N41" s="18"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
-      <c r="U41" s="5"/>
-      <c r="V41" s="5"/>
-      <c r="W41" s="5"/>
-      <c r="X41" s="5"/>
-      <c r="Y41" s="5"/>
-      <c r="Z41" s="5"/>
-      <c r="AA41" s="5"/>
-    </row>
-    <row r="42" spans="1:27" ht="30.75">
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3"/>
+      <c r="T41" s="3"/>
+      <c r="U41" s="3"/>
+      <c r="V41" s="3"/>
+      <c r="W41" s="3"/>
+      <c r="X41" s="3"/>
+      <c r="Y41" s="3"/>
+      <c r="Z41" s="3"/>
+      <c r="AA41" s="3"/>
+    </row>
+    <row r="42" spans="1:27" ht="26.25">
       <c r="A42" s="37" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>97</v>
+        <v>141</v>
       </c>
       <c r="C42" s="54" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
-      <c r="D42" s="68"/>
+      <c r="D42" s="68" t="s">
+        <v>154</v>
+      </c>
       <c r="E42" s="35"/>
       <c r="F42" s="35" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="G42" s="54"/>
-      <c r="H42" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="I42" s="54" t="s">
-        <v>99</v>
-      </c>
-      <c r="J42" s="54" t="s">
-        <v>144</v>
-      </c>
+      <c r="H42" s="35"/>
+      <c r="I42" s="54"/>
+      <c r="J42" s="54"/>
       <c r="K42" s="35"/>
       <c r="L42" s="68"/>
       <c r="M42" s="35"/>
       <c r="N42" s="18"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
-      <c r="V42" s="3"/>
-      <c r="W42" s="3"/>
-      <c r="X42" s="3"/>
-      <c r="Y42" s="3"/>
-      <c r="Z42" s="3"/>
-      <c r="AA42" s="3"/>
-    </row>
-    <row r="43" spans="1:27" ht="15.75">
-      <c r="A43" s="38"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="69"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="55"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="55"/>
-      <c r="L43" s="69"/>
-      <c r="M43" s="38"/>
-      <c r="N43" s="38"/>
-      <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
-      <c r="Q43" s="2"/>
-      <c r="R43" s="2"/>
-      <c r="S43" s="2"/>
-      <c r="T43" s="2"/>
-      <c r="U43" s="2"/>
-      <c r="V43" s="1"/>
-      <c r="W43" s="1"/>
-      <c r="X43" s="1"/>
-      <c r="Y43" s="1"/>
-      <c r="Z43" s="1"/>
-      <c r="AA43" s="1"/>
-    </row>
-    <row r="44" spans="1:27" ht="15" customHeight="1">
-      <c r="A44" s="37" t="s">
-        <v>13</v>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+      <c r="S42" s="5"/>
+      <c r="T42" s="5"/>
+      <c r="U42" s="5"/>
+      <c r="V42" s="5"/>
+      <c r="W42" s="5"/>
+      <c r="X42" s="5"/>
+      <c r="Y42" s="5"/>
+      <c r="Z42" s="5"/>
+      <c r="AA42" s="5"/>
+    </row>
+    <row r="43" spans="1:27" ht="30.75">
+      <c r="A43" s="37" t="s">
+        <v>101</v>
       </c>
-      <c r="B44" s="37" t="s">
-        <v>100</v>
+      <c r="B43" s="37" t="s">
+        <v>97</v>
       </c>
-      <c r="C44" s="56" t="s">
-        <v>152</v>
+      <c r="C43" s="54" t="s">
+        <v>143</v>
       </c>
-      <c r="D44" s="70"/>
-      <c r="E44" s="37" t="s">
-        <v>17</v>
+      <c r="D43" s="68"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35" t="s">
+        <v>33</v>
       </c>
-      <c r="F44" s="37"/>
-      <c r="G44" s="56"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="56"/>
-      <c r="J44" s="56"/>
-      <c r="K44" s="37"/>
-      <c r="L44" s="70"/>
-      <c r="M44" s="37"/>
-      <c r="N44" s="37"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="I43" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="J43" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="K43" s="35"/>
+      <c r="L43" s="68"/>
+      <c r="M43" s="35"/>
+      <c r="N43" s="18"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="U43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="3"/>
+      <c r="X43" s="3"/>
+      <c r="Y43" s="3"/>
+      <c r="Z43" s="3"/>
+      <c r="AA43" s="3"/>
+    </row>
+    <row r="44" spans="1:27" ht="15.75">
+      <c r="A44" s="38"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="55"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="55"/>
+      <c r="L44" s="69"/>
+      <c r="M44" s="38"/>
+      <c r="N44" s="38"/>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
@@ -2733,38 +2750,36 @@
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
-      <c r="V44" s="2"/>
-      <c r="W44" s="2"/>
-      <c r="X44" s="2"/>
-      <c r="Y44" s="2"/>
-      <c r="Z44" s="2"/>
-      <c r="AA44" s="2"/>
-    </row>
-    <row r="45" spans="1:27" ht="30.75">
+      <c r="V44" s="1"/>
+      <c r="W44" s="1"/>
+      <c r="X44" s="1"/>
+      <c r="Y44" s="1"/>
+      <c r="Z44" s="1"/>
+      <c r="AA44" s="1"/>
+    </row>
+    <row r="45" spans="1:27" ht="15" customHeight="1">
       <c r="A45" s="37" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
-      <c r="C45" s="54" t="s">
-        <v>103</v>
+      <c r="C45" s="56" t="s">
+        <v>152</v>
       </c>
-      <c r="D45" s="68"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="54"/>
-      <c r="H45" s="35" t="s">
-        <v>98</v>
+      <c r="D45" s="70"/>
+      <c r="E45" s="37" t="s">
+        <v>17</v>
       </c>
-      <c r="I45" s="54" t="s">
-        <v>99</v>
-      </c>
-      <c r="J45" s="54"/>
-      <c r="K45" s="35"/>
-      <c r="L45" s="68"/>
-      <c r="M45" s="35"/>
-      <c r="N45" s="35"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="56"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="70"/>
+      <c r="M45" s="37"/>
+      <c r="N45" s="37"/>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
@@ -2779,25 +2794,25 @@
       <c r="Z45" s="2"/>
       <c r="AA45" s="2"/>
     </row>
-    <row r="46" spans="1:27" ht="15.75">
+    <row r="46" spans="1:27" ht="30.75">
       <c r="A46" s="37" t="s">
         <v>101</v>
       </c>
       <c r="B46" s="37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C46" s="54" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D46" s="68"/>
       <c r="E46" s="35"/>
       <c r="F46" s="35"/>
       <c r="G46" s="54"/>
       <c r="H46" s="35" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="I46" s="54" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="J46" s="54"/>
       <c r="K46" s="35"/>
@@ -2818,23 +2833,31 @@
       <c r="Z46" s="2"/>
       <c r="AA46" s="2"/>
     </row>
-    <row r="47" spans="1:27" ht="12.75" customHeight="1">
+    <row r="47" spans="1:27" ht="15.75">
       <c r="A47" s="37" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
-      <c r="B47" s="37"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="70"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="56"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="56"/>
-      <c r="J47" s="56"/>
-      <c r="K47" s="37"/>
-      <c r="L47" s="70"/>
-      <c r="M47" s="37"/>
-      <c r="N47" s="37"/>
+      <c r="B47" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="D47" s="68"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="54"/>
+      <c r="H47" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="I47" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="J47" s="54"/>
+      <c r="K47" s="35"/>
+      <c r="L47" s="68"/>
+      <c r="M47" s="35"/>
+      <c r="N47" s="35"/>
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
@@ -2850,18 +2873,22 @@
       <c r="AA47" s="2"/>
     </row>
     <row r="48" spans="1:27" ht="12.75" customHeight="1">
-      <c r="A48" s="38"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="69"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="55"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="55"/>
-      <c r="L48" s="69"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
+      <c r="A48" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="37"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="70"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="56"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="56"/>
+      <c r="J48" s="56"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="70"/>
+      <c r="M48" s="37"/>
+      <c r="N48" s="37"/>
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
@@ -2876,33 +2903,19 @@
       <c r="Z48" s="2"/>
       <c r="AA48" s="2"/>
     </row>
-    <row r="49" spans="1:27" ht="30.75">
-      <c r="A49" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="B49" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="C49" s="54" t="s">
-        <v>148</v>
-      </c>
-      <c r="D49" s="68"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G49" s="54"/>
-      <c r="H49" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="I49" s="54" t="s">
-        <v>149</v>
-      </c>
-      <c r="J49" s="54"/>
-      <c r="K49" s="54"/>
-      <c r="L49" s="68"/>
-      <c r="M49" s="54"/>
-      <c r="N49" s="54"/>
+    <row r="49" spans="1:27" ht="12.75" customHeight="1">
+      <c r="A49" s="38"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="55"/>
+      <c r="D49" s="69"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="55"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="55"/>
+      <c r="L49" s="69"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
@@ -2917,26 +2930,28 @@
       <c r="Z49" s="2"/>
       <c r="AA49" s="2"/>
     </row>
-    <row r="50" spans="1:27" ht="15.75">
+    <row r="50" spans="1:27" ht="30.75">
       <c r="A50" s="37" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C50" s="54" t="s">
-        <v>111</v>
+        <v>148</v>
       </c>
       <c r="D50" s="68"/>
       <c r="E50" s="35"/>
       <c r="F50" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="G50" s="54" t="s">
-        <v>151</v>
+      <c r="G50" s="54"/>
+      <c r="H50" s="35" t="s">
+        <v>98</v>
       </c>
-      <c r="H50" s="35"/>
-      <c r="I50" s="54"/>
+      <c r="I50" s="54" t="s">
+        <v>149</v>
+      </c>
       <c r="J50" s="54"/>
       <c r="K50" s="54"/>
       <c r="L50" s="68"/>
@@ -2956,30 +2971,26 @@
       <c r="Z50" s="2"/>
       <c r="AA50" s="2"/>
     </row>
-    <row r="51" spans="1:27" ht="26.25">
+    <row r="51" spans="1:27" ht="15.75">
       <c r="A51" s="37" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B51" s="37" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C51" s="54" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
-      <c r="D51" s="68" t="s">
-        <v>113</v>
-      </c>
+      <c r="D51" s="68"/>
       <c r="E51" s="35"/>
       <c r="F51" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="G51" s="54"/>
-      <c r="H51" s="35" t="s">
-        <v>98</v>
+      <c r="G51" s="54" t="s">
+        <v>151</v>
       </c>
-      <c r="I51" s="54" t="s">
-        <v>149</v>
-      </c>
+      <c r="H51" s="35"/>
+      <c r="I51" s="54"/>
       <c r="J51" s="54"/>
       <c r="K51" s="54"/>
       <c r="L51" s="68"/>
@@ -2999,23 +3010,35 @@
       <c r="Z51" s="2"/>
       <c r="AA51" s="2"/>
     </row>
-    <row r="52" spans="1:27" ht="12.75" customHeight="1">
+    <row r="52" spans="1:27" ht="26.25">
       <c r="A52" s="37" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
-      <c r="B52" s="37"/>
-      <c r="C52" s="56"/>
-      <c r="D52" s="59"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="56"/>
-      <c r="H52" s="37"/>
-      <c r="I52" s="56"/>
-      <c r="J52" s="56"/>
-      <c r="K52" s="37"/>
-      <c r="L52" s="70"/>
-      <c r="M52" s="37"/>
-      <c r="N52" s="37"/>
+      <c r="B52" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C52" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="D52" s="68" t="s">
+        <v>113</v>
+      </c>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G52" s="54"/>
+      <c r="H52" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="I52" s="54" t="s">
+        <v>149</v>
+      </c>
+      <c r="J52" s="54"/>
+      <c r="K52" s="54"/>
+      <c r="L52" s="68"/>
+      <c r="M52" s="54"/>
+      <c r="N52" s="54"/>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
@@ -3031,20 +3054,22 @@
       <c r="AA52" s="2"/>
     </row>
     <row r="53" spans="1:27" ht="12.75" customHeight="1">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="49"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="49"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="49"/>
-      <c r="J53" s="49"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="49"/>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
+      <c r="A53" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="37"/>
+      <c r="C53" s="56"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="56"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="56"/>
+      <c r="J53" s="56"/>
+      <c r="K53" s="37"/>
+      <c r="L53" s="70"/>
+      <c r="M53" s="37"/>
+      <c r="N53" s="37"/>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
@@ -8221,7 +8246,7 @@
       <c r="Z231" s="2"/>
       <c r="AA231" s="2"/>
     </row>
-    <row r="232" spans="1:27" ht="15.75" customHeight="1">
+    <row r="232" spans="1:27" ht="12.75" customHeight="1">
       <c r="A232" s="2"/>
       <c r="B232" s="2"/>
       <c r="C232" s="49"/>
@@ -30696,7 +30721,7 @@
       <c r="Z1006" s="2"/>
       <c r="AA1006" s="2"/>
     </row>
-    <row r="1007" spans="1:27" ht="15" customHeight="1">
+    <row r="1007" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1007" s="2"/>
       <c r="B1007" s="2"/>
       <c r="C1007" s="49"/>
@@ -30709,6 +30734,21 @@
       <c r="J1007" s="49"/>
       <c r="K1007" s="2"/>
       <c r="L1007" s="49"/>
+      <c r="M1007" s="2"/>
+      <c r="N1007" s="2"/>
+      <c r="O1007" s="2"/>
+      <c r="P1007" s="2"/>
+      <c r="Q1007" s="2"/>
+      <c r="R1007" s="2"/>
+      <c r="S1007" s="2"/>
+      <c r="T1007" s="2"/>
+      <c r="U1007" s="2"/>
+      <c r="V1007" s="2"/>
+      <c r="W1007" s="2"/>
+      <c r="X1007" s="2"/>
+      <c r="Y1007" s="2"/>
+      <c r="Z1007" s="2"/>
+      <c r="AA1007" s="2"/>
     </row>
     <row r="1008" spans="1:27" ht="15" customHeight="1">
       <c r="A1008" s="2"/>
@@ -30934,6 +30974,20 @@
       <c r="K1023" s="2"/>
       <c r="L1023" s="49"/>
     </row>
+    <row r="1024" spans="1:12" ht="15" customHeight="1">
+      <c r="A1024" s="2"/>
+      <c r="B1024" s="2"/>
+      <c r="C1024" s="49"/>
+      <c r="D1024" s="2"/>
+      <c r="E1024" s="2"/>
+      <c r="F1024" s="2"/>
+      <c r="G1024" s="49"/>
+      <c r="H1024" s="2"/>
+      <c r="I1024" s="49"/>
+      <c r="J1024" s="49"/>
+      <c r="K1024" s="2"/>
+      <c r="L1024" s="49"/>
+    </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -30944,9 +30998,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z991"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -31677,9 +31731,15 @@
       <c r="Z22" s="6"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
+      <c r="A23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>161</v>
+      </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>

</xml_diff>

<commit_message>
Making constraint changes for VMMC no. in the enroll form, new role added for task viewing
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/enroll.xlsx
+++ b/config/itech-aurum/forms/app/enroll.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-81\itech-aurum\forms\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-99\itech-aurum\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A705671D-BCC8-47EE-8CAD-A7FACA4F06F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A96860-251B-43B7-B724-7B6648529F1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -524,13 +524,13 @@
     <t>instance::tag</t>
   </si>
   <si>
-    <t>regex(., '^[A-Z]{2}[0-9]{4}$')</t>
-  </si>
-  <si>
     <t>e.g. 0001</t>
   </si>
   <si>
     <t>e.g. WM0000</t>
+  </si>
+  <si>
+    <t>regex(., '^[A-Za-z0-9]{1,7}$')</t>
   </si>
 </sst>
 </file>
@@ -1125,10 +1125,10 @@
   <dimension ref="A1:AA1024"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J34" sqref="J34"/>
+      <selection pane="bottomRight" activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -2335,13 +2335,13 @@
       </c>
       <c r="G33" s="71"/>
       <c r="H33" s="36" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="I33" s="52" t="s">
         <v>162</v>
       </c>
       <c r="J33" s="52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K33" s="17"/>
       <c r="L33" s="68"/>
@@ -2386,7 +2386,7 @@
         <v>163</v>
       </c>
       <c r="J34" s="52" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K34" s="17"/>
       <c r="L34" s="68"/>

</xml_diff>

<commit_message>
Making constraint changes for 2WT study no. in the enroll form
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/enroll.xlsx
+++ b/config/itech-aurum/forms/app/enroll.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-99\itech-aurum\forms\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-108\itech-aurum\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A96860-251B-43B7-B724-7B6648529F1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3AA214-CD6E-43D2-9FF3-CF2C1EAB4935}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,9 +509,6 @@
     <t>select_multiple yes</t>
   </si>
   <si>
-    <t>regex(., '^[0-9]+$')</t>
-  </si>
-  <si>
     <t>Please enter valid VMMC client name</t>
   </si>
   <si>
@@ -531,6 +528,9 @@
   </si>
   <si>
     <t>regex(., '^[A-Za-z0-9]{1,7}$')</t>
+  </si>
+  <si>
+    <t>regex(., '^[0-9]{4}$')</t>
   </si>
 </sst>
 </file>
@@ -1125,10 +1125,10 @@
   <dimension ref="A1:AA1024"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H33" sqref="H33"/>
+      <selection pane="bottomRight" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -1196,7 +1196,7 @@
         <v>12</v>
       </c>
       <c r="O1" s="33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P1" s="31"/>
       <c r="Q1" s="31"/>
@@ -2295,7 +2295,7 @@
         <v>58</v>
       </c>
       <c r="I32" s="53" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J32" s="53"/>
       <c r="K32" s="19"/>
@@ -2335,13 +2335,13 @@
       </c>
       <c r="G33" s="71"/>
       <c r="H33" s="36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I33" s="52" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J33" s="52" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K33" s="17"/>
       <c r="L33" s="68"/>
@@ -2380,13 +2380,13 @@
       </c>
       <c r="G34" s="54"/>
       <c r="H34" s="36" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="I34" s="52" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J34" s="52" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K34" s="17"/>
       <c r="L34" s="68"/>

</xml_diff>

<commit_message>
Add a context in contact-summary and check it in the enroll form to avoid editing #108
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/enroll.xlsx
+++ b/config/itech-aurum/forms/app/enroll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-108\itech-aurum\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3AA214-CD6E-43D2-9FF3-CF2C1EAB4935}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9806D289-A2CB-4589-BABF-6C0E41F022BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="178">
   <si>
     <t>type</t>
   </si>
@@ -532,6 +532,36 @@
   <si>
     <t>regex(., '^[0-9]{4}$')</t>
   </si>
+  <si>
+    <t>ctx</t>
+  </si>
+  <si>
+    <t>instance('contact-summary')/context/isContact</t>
+  </si>
+  <si>
+    <t>editing</t>
+  </si>
+  <si>
+    <t>if(${ctx} = 'yes', 'no', 'yes')</t>
+  </si>
+  <si>
+    <t>forbid</t>
+  </si>
+  <si>
+    <t>../editing = 'yes'</t>
+  </si>
+  <si>
+    <t>n_edit</t>
+  </si>
+  <si>
+    <t>&lt;span style="color:red;"&gt;You can not edit this form. Please cancel.&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>no_edit</t>
+  </si>
+  <si>
+    <t>. = 1</t>
+  </si>
 </sst>
 </file>
 
@@ -662,7 +692,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -741,6 +771,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -769,7 +811,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -907,6 +949,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1122,13 +1172,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA1024"/>
+  <dimension ref="A1:AA1031"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H34" sqref="H34"/>
+      <selection pane="bottomRight" activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -1950,32 +2000,28 @@
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" spans="1:27" ht="15.75">
-      <c r="A23" s="72" t="s">
-        <v>13</v>
+    <row r="23" spans="1:27" ht="12.75" customHeight="1">
+      <c r="A23" s="77" t="s">
+        <v>42</v>
       </c>
-      <c r="B23" s="72" t="s">
-        <v>46</v>
+      <c r="B23" s="77" t="s">
+        <v>168</v>
       </c>
-      <c r="C23" s="51" t="s">
-        <v>40</v>
+      <c r="C23" s="78"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="80"/>
+      <c r="I23" s="78"/>
+      <c r="J23" s="78"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="80" t="s">
+        <v>169</v>
       </c>
-      <c r="D23" s="65"/>
-      <c r="E23" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="23"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="65"/>
-      <c r="M23" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
+      <c r="M23" s="80"/>
+      <c r="N23" s="80"/>
+      <c r="O23" s="80"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
@@ -1989,30 +2035,28 @@
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" spans="1:27" ht="15.75">
-      <c r="A24" s="17" t="s">
-        <v>13</v>
+    <row r="24" spans="1:27" ht="12.75" customHeight="1">
+      <c r="A24" s="77" t="s">
+        <v>42</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>38</v>
+      <c r="B24" s="77" t="s">
+        <v>170</v>
       </c>
-      <c r="C24" s="74" t="s">
-        <v>40</v>
+      <c r="C24" s="78"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="78"/>
+      <c r="J24" s="78"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="80" t="s">
+        <v>171</v>
       </c>
-      <c r="D24" s="75"/>
-      <c r="E24" s="73" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" s="73"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="74"/>
-      <c r="J24" s="74"/>
-      <c r="K24" s="73"/>
-      <c r="L24" s="75"/>
-      <c r="M24" s="73"/>
-      <c r="N24" s="73"/>
-      <c r="O24" s="73"/>
+      <c r="M24" s="80"/>
+      <c r="N24" s="80"/>
+      <c r="O24" s="80"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
@@ -2026,32 +2070,30 @@
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" spans="1:27" ht="15.75">
-      <c r="A25" s="17" t="s">
-        <v>42</v>
+    <row r="25" spans="1:27" ht="12.75" customHeight="1">
+      <c r="A25" s="77" t="s">
+        <v>13</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>30</v>
+      <c r="B25" s="77" t="s">
+        <v>172</v>
       </c>
-      <c r="C25" s="74" t="s">
-        <v>40</v>
+      <c r="C25" s="78"/>
+      <c r="D25" s="79" t="s">
+        <v>173</v>
       </c>
-      <c r="D25" s="75"/>
-      <c r="E25" s="73" t="s">
-        <v>21</v>
+      <c r="E25" s="80" t="s">
+        <v>17</v>
       </c>
-      <c r="F25" s="73"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="74"/>
-      <c r="J25" s="74"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="75" t="s">
-        <v>54</v>
-      </c>
-      <c r="M25" s="73"/>
-      <c r="N25" s="73"/>
-      <c r="O25" s="73"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="80"/>
+      <c r="I25" s="78"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="79"/>
+      <c r="L25" s="80"/>
+      <c r="M25" s="80"/>
+      <c r="N25" s="80"/>
+      <c r="O25" s="80"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
@@ -2065,30 +2107,28 @@
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
     </row>
-    <row r="26" spans="1:27" ht="15.75">
-      <c r="A26" s="17" t="s">
-        <v>13</v>
+    <row r="26" spans="1:27" ht="12.75" customHeight="1">
+      <c r="A26" s="77" t="s">
+        <v>81</v>
       </c>
-      <c r="B26" s="17" t="s">
-        <v>38</v>
+      <c r="B26" s="77" t="s">
+        <v>174</v>
       </c>
-      <c r="C26" s="74" t="s">
-        <v>40</v>
+      <c r="C26" s="78" t="s">
+        <v>175</v>
       </c>
-      <c r="D26" s="75"/>
-      <c r="E26" s="73" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="73"/>
-      <c r="G26" s="74"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="74"/>
-      <c r="J26" s="74"/>
-      <c r="K26" s="73"/>
-      <c r="L26" s="75"/>
-      <c r="M26" s="73"/>
-      <c r="N26" s="73"/>
-      <c r="O26" s="73"/>
+      <c r="D26" s="79"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="80"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="78"/>
+      <c r="K26" s="79"/>
+      <c r="L26" s="80"/>
+      <c r="M26" s="80"/>
+      <c r="N26" s="80"/>
+      <c r="O26" s="80"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
@@ -2102,32 +2142,34 @@
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
     </row>
-    <row r="27" spans="1:27" ht="15.75">
-      <c r="A27" s="17" t="s">
-        <v>42</v>
+    <row r="27" spans="1:27" ht="12.75" customHeight="1">
+      <c r="A27" s="77" t="s">
+        <v>97</v>
       </c>
-      <c r="B27" s="17" t="s">
-        <v>30</v>
+      <c r="B27" s="77" t="s">
+        <v>176</v>
       </c>
-      <c r="C27" s="74" t="s">
+      <c r="C27" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="75"/>
-      <c r="E27" s="73" t="s">
+      <c r="D27" s="79"/>
+      <c r="E27" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="F27" s="73"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="73"/>
-      <c r="I27" s="74"/>
-      <c r="J27" s="74"/>
-      <c r="K27" s="73"/>
-      <c r="L27" s="75" t="s">
-        <v>55</v>
+      <c r="F27" s="80"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="78" t="s">
+        <v>177</v>
       </c>
-      <c r="M27" s="73"/>
-      <c r="N27" s="73"/>
-      <c r="O27" s="73"/>
+      <c r="I27" s="78"/>
+      <c r="J27" s="78"/>
+      <c r="K27" s="79">
+        <v>0</v>
+      </c>
+      <c r="L27" s="80"/>
+      <c r="M27" s="80"/>
+      <c r="N27" s="80"/>
+      <c r="O27" s="80"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
@@ -2142,23 +2184,23 @@
       <c r="AA27" s="1"/>
     </row>
     <row r="28" spans="1:27" ht="12.75" customHeight="1">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="73"/>
-      <c r="I28" s="74"/>
-      <c r="J28" s="74"/>
-      <c r="K28" s="73"/>
-      <c r="L28" s="75"/>
-      <c r="M28" s="73"/>
-      <c r="N28" s="73"/>
-      <c r="O28" s="73"/>
+      <c r="B28" s="77"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="79"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="80"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="80"/>
+      <c r="I28" s="78"/>
+      <c r="J28" s="78"/>
+      <c r="K28" s="80"/>
+      <c r="L28" s="79"/>
+      <c r="M28" s="80"/>
+      <c r="N28" s="80"/>
+      <c r="O28" s="80"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
@@ -2173,23 +2215,21 @@
       <c r="AA28" s="1"/>
     </row>
     <row r="29" spans="1:27" ht="12.75" customHeight="1">
-      <c r="A29" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="73"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="74"/>
-      <c r="H29" s="73"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="74"/>
-      <c r="K29" s="73"/>
-      <c r="L29" s="75"/>
-      <c r="M29" s="73"/>
-      <c r="N29" s="73"/>
-      <c r="O29" s="73"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="63"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
@@ -2204,29 +2244,31 @@
       <c r="AA29" s="1"/>
     </row>
     <row r="30" spans="1:27" ht="15.75">
-      <c r="A30" s="23" t="s">
-        <v>42</v>
+      <c r="A30" s="72" t="s">
+        <v>13</v>
       </c>
-      <c r="B30" s="23" t="s">
-        <v>0</v>
+      <c r="B30" s="72" t="s">
+        <v>46</v>
       </c>
-      <c r="C30" s="52" t="s">
-        <v>56</v>
+      <c r="C30" s="51" t="s">
+        <v>40</v>
       </c>
-      <c r="D30" s="66"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="66" t="s">
-        <v>57</v>
+      <c r="D30" s="65"/>
+      <c r="E30" s="23" t="s">
+        <v>17</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="65"/>
+      <c r="M30" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
@@ -2241,27 +2283,29 @@
       <c r="AA30" s="1"/>
     </row>
     <row r="31" spans="1:27" ht="15.75">
-      <c r="A31" s="23" t="s">
-        <v>42</v>
+      <c r="A31" s="17" t="s">
+        <v>13</v>
       </c>
-      <c r="B31" s="23" t="s">
-        <v>152</v>
+      <c r="B31" s="17" t="s">
+        <v>38</v>
       </c>
-      <c r="C31" s="52"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="66" t="s">
-        <v>153</v>
+      <c r="C31" s="74" t="s">
+        <v>40</v>
       </c>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" s="73"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="73"/>
+      <c r="I31" s="74"/>
+      <c r="J31" s="74"/>
+      <c r="K31" s="73"/>
+      <c r="L31" s="75"/>
+      <c r="M31" s="73"/>
+      <c r="N31" s="73"/>
+      <c r="O31" s="73"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
@@ -2275,419 +2319,399 @@
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
     </row>
-    <row r="32" spans="1:27" ht="30.75">
-      <c r="A32" s="24" t="s">
+    <row r="32" spans="1:27" ht="15.75">
+      <c r="A32" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="74" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="75"/>
+      <c r="E32" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" s="73"/>
+      <c r="G32" s="74"/>
+      <c r="H32" s="73"/>
+      <c r="I32" s="74"/>
+      <c r="J32" s="74"/>
+      <c r="K32" s="73"/>
+      <c r="L32" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="M32" s="73"/>
+      <c r="N32" s="73"/>
+      <c r="O32" s="73"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+    </row>
+    <row r="33" spans="1:27" ht="15.75">
+      <c r="A33" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="74" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="75"/>
+      <c r="E33" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="73"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="73"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="74"/>
+      <c r="K33" s="73"/>
+      <c r="L33" s="75"/>
+      <c r="M33" s="73"/>
+      <c r="N33" s="73"/>
+      <c r="O33" s="73"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="1"/>
+    </row>
+    <row r="34" spans="1:27" ht="15.75">
+      <c r="A34" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="74" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="75"/>
+      <c r="E34" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="73"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="74"/>
+      <c r="J34" s="74"/>
+      <c r="K34" s="73"/>
+      <c r="L34" s="75" t="s">
+        <v>55</v>
+      </c>
+      <c r="M34" s="73"/>
+      <c r="N34" s="73"/>
+      <c r="O34" s="73"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+      <c r="Z34" s="1"/>
+      <c r="AA34" s="1"/>
+    </row>
+    <row r="35" spans="1:27" ht="12.75" customHeight="1">
+      <c r="A35" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="17"/>
+      <c r="C35" s="74"/>
+      <c r="D35" s="75"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="74"/>
+      <c r="H35" s="73"/>
+      <c r="I35" s="74"/>
+      <c r="J35" s="74"/>
+      <c r="K35" s="73"/>
+      <c r="L35" s="75"/>
+      <c r="M35" s="73"/>
+      <c r="N35" s="73"/>
+      <c r="O35" s="73"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+      <c r="Y35" s="1"/>
+      <c r="Z35" s="1"/>
+      <c r="AA35" s="1"/>
+    </row>
+    <row r="36" spans="1:27" ht="12.75" customHeight="1">
+      <c r="A36" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="17"/>
+      <c r="C36" s="74"/>
+      <c r="D36" s="75"/>
+      <c r="E36" s="73"/>
+      <c r="F36" s="73"/>
+      <c r="G36" s="74"/>
+      <c r="H36" s="73"/>
+      <c r="I36" s="74"/>
+      <c r="J36" s="74"/>
+      <c r="K36" s="73"/>
+      <c r="L36" s="75"/>
+      <c r="M36" s="73"/>
+      <c r="N36" s="73"/>
+      <c r="O36" s="73"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1"/>
+      <c r="AA36" s="1"/>
+    </row>
+    <row r="37" spans="1:27" ht="15.75">
+      <c r="A37" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="66"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1"/>
+      <c r="AA37" s="1"/>
+    </row>
+    <row r="38" spans="1:27" ht="15.75">
+      <c r="A38" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="C38" s="52"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="52"/>
+      <c r="J38" s="52"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="66" t="s">
+        <v>153</v>
+      </c>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="1"/>
+    </row>
+    <row r="39" spans="1:27" ht="30.75">
+      <c r="A39" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B39" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C39" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="67"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18" t="s">
+      <c r="D39" s="67"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="53"/>
-      <c r="H32" s="18" t="s">
+      <c r="G39" s="53"/>
+      <c r="H39" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="I32" s="53" t="s">
+      <c r="I39" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="J32" s="53"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="67"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
-      <c r="S32" s="3"/>
-      <c r="T32" s="3"/>
-      <c r="U32" s="3"/>
-      <c r="V32" s="3"/>
-      <c r="W32" s="3"/>
-      <c r="X32" s="3"/>
-      <c r="Y32" s="3"/>
-      <c r="Z32" s="3"/>
-      <c r="AA32" s="3"/>
-    </row>
-    <row r="33" spans="1:27" ht="30.75">
-      <c r="A33" s="25" t="s">
+      <c r="J39" s="53"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="67"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+      <c r="Y39" s="3"/>
+      <c r="Z39" s="3"/>
+      <c r="AA39" s="3"/>
+    </row>
+    <row r="40" spans="1:27" ht="30.75">
+      <c r="A40" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B40" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="54" t="s">
+      <c r="C40" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="68"/>
-      <c r="E33" s="21" t="s">
+      <c r="D40" s="68"/>
+      <c r="E40" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F40" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G33" s="71"/>
-      <c r="H33" s="36" t="s">
+      <c r="G40" s="71"/>
+      <c r="H40" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="I33" s="52" t="s">
+      <c r="I40" s="52" t="s">
         <v>161</v>
       </c>
-      <c r="J33" s="52" t="s">
+      <c r="J40" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="K33" s="17"/>
-      <c r="L33" s="68"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="20"/>
-      <c r="O33" s="20"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-      <c r="T33" s="1"/>
-      <c r="U33" s="1"/>
-      <c r="V33" s="1"/>
-      <c r="W33" s="1"/>
-      <c r="X33" s="4"/>
-      <c r="Y33" s="4"/>
-      <c r="Z33" s="1"/>
-      <c r="AA33" s="1"/>
-    </row>
-    <row r="34" spans="1:27" ht="30.75">
-      <c r="A34" s="37" t="s">
+      <c r="K40" s="17"/>
+      <c r="L40" s="68"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="20"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
+      <c r="X40" s="4"/>
+      <c r="Y40" s="4"/>
+      <c r="Z40" s="1"/>
+      <c r="AA40" s="1"/>
+    </row>
+    <row r="41" spans="1:27" ht="30.75">
+      <c r="A41" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="37" t="s">
+      <c r="B41" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="54" t="s">
+      <c r="C41" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="68"/>
-      <c r="E34" s="36" t="s">
+      <c r="D41" s="68"/>
+      <c r="E41" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F34" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G34" s="54"/>
-      <c r="H34" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="I34" s="52" t="s">
-        <v>162</v>
-      </c>
-      <c r="J34" s="52" t="s">
-        <v>164</v>
-      </c>
-      <c r="K34" s="17"/>
-      <c r="L34" s="68"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="20"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
-      <c r="T34" s="1"/>
-      <c r="U34" s="1"/>
-      <c r="V34" s="1"/>
-      <c r="W34" s="1"/>
-      <c r="X34" s="4"/>
-      <c r="Y34" s="4"/>
-      <c r="Z34" s="1"/>
-      <c r="AA34" s="1"/>
-    </row>
-    <row r="35" spans="1:27" ht="30.75">
-      <c r="A35" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="B35" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="C35" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" s="68"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="54"/>
-      <c r="J35" s="54"/>
-      <c r="K35" s="35"/>
-      <c r="L35" s="68"/>
-      <c r="M35" s="35"/>
-      <c r="N35" s="18"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="3"/>
-      <c r="Q35" s="3"/>
-      <c r="R35" s="3"/>
-      <c r="S35" s="3"/>
-      <c r="T35" s="3"/>
-      <c r="U35" s="3"/>
-      <c r="V35" s="3"/>
-      <c r="W35" s="3"/>
-      <c r="X35" s="3"/>
-      <c r="Y35" s="3"/>
-      <c r="Z35" s="1"/>
-      <c r="AA35" s="1"/>
-    </row>
-    <row r="36" spans="1:27" ht="15.75">
-      <c r="A36" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="B36" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C36" s="54" t="s">
-        <v>85</v>
-      </c>
-      <c r="D36" s="68"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G36" s="54" t="s">
-        <v>149</v>
-      </c>
-      <c r="H36" s="35"/>
-      <c r="I36" s="54"/>
-      <c r="J36" s="54"/>
-      <c r="K36" s="35"/>
-      <c r="L36" s="68"/>
-      <c r="M36" s="35"/>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
-      <c r="R36" s="3"/>
-      <c r="S36" s="3"/>
-      <c r="T36" s="3"/>
-      <c r="U36" s="3"/>
-      <c r="V36" s="3"/>
-      <c r="W36" s="3"/>
-      <c r="X36" s="3"/>
-      <c r="Y36" s="3"/>
-      <c r="Z36" s="1"/>
-      <c r="AA36" s="1"/>
-    </row>
-    <row r="37" spans="1:27" ht="15.75">
-      <c r="A37" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="B37" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="C37" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="D37" s="68"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G37" s="54"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="54"/>
-      <c r="J37" s="54"/>
-      <c r="K37" s="35"/>
-      <c r="L37" s="68"/>
-      <c r="M37" s="35"/>
-      <c r="N37" s="20"/>
-      <c r="O37" s="20"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-      <c r="S37" s="1"/>
-      <c r="T37" s="1"/>
-      <c r="U37" s="1"/>
-      <c r="V37" s="1"/>
-      <c r="W37" s="1"/>
-      <c r="X37" s="4"/>
-      <c r="Y37" s="4"/>
-      <c r="Z37" s="1"/>
-      <c r="AA37" s="1"/>
-    </row>
-    <row r="38" spans="1:27" ht="30.75">
-      <c r="A38" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="54" t="s">
-        <v>89</v>
-      </c>
-      <c r="D38" s="68"/>
-      <c r="E38" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="F38" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G38" s="54"/>
-      <c r="H38" s="35" t="s">
-        <v>158</v>
-      </c>
-      <c r="I38" s="54" t="s">
-        <v>154</v>
-      </c>
-      <c r="J38" s="54" t="s">
-        <v>155</v>
-      </c>
-      <c r="K38" s="35"/>
-      <c r="L38" s="68"/>
-      <c r="M38" s="35"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
-      <c r="S38" s="1"/>
-      <c r="T38" s="1"/>
-      <c r="U38" s="1"/>
-      <c r="V38" s="1"/>
-      <c r="W38" s="1"/>
-      <c r="X38" s="4"/>
-      <c r="Y38" s="4"/>
-      <c r="Z38" s="1"/>
-      <c r="AA38" s="1"/>
-    </row>
-    <row r="39" spans="1:27" ht="15.75">
-      <c r="A39" s="37" t="s">
-        <v>159</v>
-      </c>
-      <c r="B39" s="37" t="s">
-        <v>156</v>
-      </c>
-      <c r="C39" s="54" t="s">
-        <v>40</v>
-      </c>
-      <c r="D39" s="68"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="54"/>
-      <c r="H39" s="35"/>
-      <c r="I39" s="54"/>
-      <c r="J39" s="54"/>
-      <c r="K39" s="35"/>
-      <c r="L39" s="68"/>
-      <c r="M39" s="35"/>
-      <c r="N39" s="20"/>
-      <c r="O39" s="20"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-      <c r="S39" s="1"/>
-      <c r="T39" s="1"/>
-      <c r="U39" s="1"/>
-      <c r="V39" s="1"/>
-      <c r="W39" s="1"/>
-      <c r="X39" s="4"/>
-      <c r="Y39" s="4"/>
-      <c r="Z39" s="1"/>
-      <c r="AA39" s="1"/>
-    </row>
-    <row r="40" spans="1:27" ht="30.75">
-      <c r="A40" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B40" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="54" t="s">
-        <v>63</v>
-      </c>
-      <c r="D40" s="68"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G40" s="54"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="54"/>
-      <c r="J40" s="54"/>
-      <c r="K40" s="35"/>
-      <c r="L40" s="68"/>
-      <c r="M40" s="35"/>
-      <c r="N40" s="17"/>
-      <c r="O40" s="17"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
-      <c r="S40" s="2"/>
-      <c r="T40" s="2"/>
-      <c r="U40" s="2"/>
-      <c r="V40" s="1"/>
-      <c r="W40" s="1"/>
-      <c r="X40" s="1"/>
-      <c r="Y40" s="1"/>
-      <c r="Z40" s="1"/>
-      <c r="AA40" s="1"/>
-    </row>
-    <row r="41" spans="1:27" ht="15.75">
-      <c r="A41" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="B41" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="C41" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" s="68"/>
-      <c r="E41" s="35"/>
       <c r="F41" s="35" t="s">
         <v>33</v>
       </c>
       <c r="G41" s="54"/>
-      <c r="H41" s="35"/>
-      <c r="I41" s="54"/>
-      <c r="J41" s="54"/>
-      <c r="K41" s="35"/>
+      <c r="H41" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="I41" s="52" t="s">
+        <v>162</v>
+      </c>
+      <c r="J41" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="K41" s="17"/>
       <c r="L41" s="68"/>
-      <c r="M41" s="35"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
-      <c r="T41" s="3"/>
-      <c r="U41" s="3"/>
-      <c r="V41" s="3"/>
-      <c r="W41" s="3"/>
-      <c r="X41" s="3"/>
-      <c r="Y41" s="3"/>
-      <c r="Z41" s="3"/>
-      <c r="AA41" s="3"/>
-    </row>
-    <row r="42" spans="1:27" ht="26.25">
+      <c r="M41" s="20"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="20"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
+      <c r="X41" s="4"/>
+      <c r="Y41" s="4"/>
+      <c r="Z41" s="1"/>
+      <c r="AA41" s="1"/>
+    </row>
+    <row r="42" spans="1:27" ht="30.75">
       <c r="A42" s="37" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="C42" s="54" t="s">
-        <v>138</v>
+        <v>82</v>
       </c>
-      <c r="D42" s="68" t="s">
-        <v>150</v>
-      </c>
+      <c r="D42" s="68"/>
       <c r="E42" s="35"/>
-      <c r="F42" s="35" t="s">
-        <v>59</v>
-      </c>
+      <c r="F42" s="35"/>
       <c r="G42" s="54"/>
       <c r="H42" s="35"/>
       <c r="I42" s="54"/>
@@ -2697,44 +2721,40 @@
       <c r="M42" s="35"/>
       <c r="N42" s="18"/>
       <c r="O42" s="18"/>
-      <c r="P42" s="5"/>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
-      <c r="U42" s="5"/>
-      <c r="V42" s="5"/>
-      <c r="W42" s="5"/>
-      <c r="X42" s="5"/>
-      <c r="Y42" s="5"/>
-      <c r="Z42" s="5"/>
-      <c r="AA42" s="5"/>
-    </row>
-    <row r="43" spans="1:27" ht="30.75">
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="U42" s="3"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="3"/>
+      <c r="X42" s="3"/>
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="1"/>
+      <c r="AA42" s="1"/>
+    </row>
+    <row r="43" spans="1:27" ht="15.75">
       <c r="A43" s="37" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C43" s="54" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
       <c r="D43" s="68"/>
       <c r="E43" s="35"/>
       <c r="F43" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="G43" s="54"/>
-      <c r="H43" s="35" t="s">
-        <v>94</v>
+      <c r="G43" s="54" t="s">
+        <v>149</v>
       </c>
-      <c r="I43" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="J43" s="54" t="s">
-        <v>140</v>
-      </c>
+      <c r="H43" s="35"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54"/>
       <c r="K43" s="35"/>
       <c r="L43" s="68"/>
       <c r="M43" s="35"/>
@@ -2750,218 +2770,248 @@
       <c r="W43" s="3"/>
       <c r="X43" s="3"/>
       <c r="Y43" s="3"/>
-      <c r="Z43" s="3"/>
-      <c r="AA43" s="3"/>
+      <c r="Z43" s="1"/>
+      <c r="AA43" s="1"/>
     </row>
     <row r="44" spans="1:27" ht="15.75">
-      <c r="A44" s="38"/>
-      <c r="B44" s="38"/>
-      <c r="C44" s="58"/>
-      <c r="D44" s="69"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="55"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="55"/>
-      <c r="L44" s="69"/>
-      <c r="M44" s="38"/>
-      <c r="N44" s="38"/>
-      <c r="O44" s="38"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="2"/>
-      <c r="R44" s="2"/>
-      <c r="S44" s="2"/>
-      <c r="T44" s="2"/>
-      <c r="U44" s="2"/>
+      <c r="A44" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" s="68"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G44" s="54"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="54"/>
+      <c r="J44" s="54"/>
+      <c r="K44" s="35"/>
+      <c r="L44" s="68"/>
+      <c r="M44" s="35"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
       <c r="V44" s="1"/>
       <c r="W44" s="1"/>
-      <c r="X44" s="1"/>
-      <c r="Y44" s="1"/>
+      <c r="X44" s="4"/>
+      <c r="Y44" s="4"/>
       <c r="Z44" s="1"/>
       <c r="AA44" s="1"/>
     </row>
-    <row r="45" spans="1:27" ht="15" customHeight="1">
+    <row r="45" spans="1:27" ht="30.75">
       <c r="A45" s="37" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>96</v>
+        <v>36</v>
       </c>
-      <c r="C45" s="56" t="s">
-        <v>148</v>
+      <c r="C45" s="54" t="s">
+        <v>89</v>
       </c>
-      <c r="D45" s="70"/>
-      <c r="E45" s="37" t="s">
-        <v>17</v>
+      <c r="D45" s="68"/>
+      <c r="E45" s="35" t="s">
+        <v>61</v>
       </c>
-      <c r="F45" s="37"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="37"/>
-      <c r="L45" s="70"/>
-      <c r="M45" s="37"/>
-      <c r="N45" s="37"/>
-      <c r="O45" s="37"/>
-      <c r="P45" s="2"/>
-      <c r="Q45" s="2"/>
-      <c r="R45" s="2"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="2"/>
-      <c r="U45" s="2"/>
-      <c r="V45" s="2"/>
-      <c r="W45" s="2"/>
-      <c r="X45" s="2"/>
-      <c r="Y45" s="2"/>
-      <c r="Z45" s="2"/>
-      <c r="AA45" s="2"/>
-    </row>
-    <row r="46" spans="1:27" ht="30.75">
+      <c r="F45" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G45" s="54"/>
+      <c r="H45" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="I45" s="54" t="s">
+        <v>154</v>
+      </c>
+      <c r="J45" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="K45" s="35"/>
+      <c r="L45" s="68"/>
+      <c r="M45" s="35"/>
+      <c r="N45" s="20"/>
+      <c r="O45" s="20"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="1"/>
+      <c r="X45" s="4"/>
+      <c r="Y45" s="4"/>
+      <c r="Z45" s="1"/>
+      <c r="AA45" s="1"/>
+    </row>
+    <row r="46" spans="1:27" ht="15.75">
       <c r="A46" s="37" t="s">
-        <v>97</v>
+        <v>159</v>
       </c>
       <c r="B46" s="37" t="s">
-        <v>98</v>
+        <v>156</v>
       </c>
       <c r="C46" s="54" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="D46" s="68"/>
       <c r="E46" s="35"/>
       <c r="F46" s="35"/>
       <c r="G46" s="54"/>
-      <c r="H46" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="I46" s="54" t="s">
-        <v>95</v>
-      </c>
+      <c r="H46" s="35"/>
+      <c r="I46" s="54"/>
       <c r="J46" s="54"/>
       <c r="K46" s="35"/>
       <c r="L46" s="68"/>
       <c r="M46" s="35"/>
-      <c r="N46" s="35"/>
-      <c r="O46" s="35"/>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="2"/>
-      <c r="R46" s="2"/>
-      <c r="S46" s="2"/>
-      <c r="T46" s="2"/>
-      <c r="U46" s="2"/>
-      <c r="V46" s="2"/>
-      <c r="W46" s="2"/>
-      <c r="X46" s="2"/>
-      <c r="Y46" s="2"/>
-      <c r="Z46" s="2"/>
-      <c r="AA46" s="2"/>
-    </row>
-    <row r="47" spans="1:27" ht="15.75">
+      <c r="N46" s="20"/>
+      <c r="O46" s="20"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
+      <c r="W46" s="1"/>
+      <c r="X46" s="4"/>
+      <c r="Y46" s="4"/>
+      <c r="Z46" s="1"/>
+      <c r="AA46" s="1"/>
+    </row>
+    <row r="47" spans="1:27" ht="30.75">
       <c r="A47" s="37" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="B47" s="37" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="C47" s="54" t="s">
-        <v>101</v>
+        <v>63</v>
       </c>
       <c r="D47" s="68"/>
       <c r="E47" s="35"/>
-      <c r="F47" s="35"/>
+      <c r="F47" s="35" t="s">
+        <v>33</v>
+      </c>
       <c r="G47" s="54"/>
-      <c r="H47" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="I47" s="54" t="s">
-        <v>103</v>
-      </c>
+      <c r="H47" s="35"/>
+      <c r="I47" s="54"/>
       <c r="J47" s="54"/>
       <c r="K47" s="35"/>
       <c r="L47" s="68"/>
       <c r="M47" s="35"/>
-      <c r="N47" s="35"/>
-      <c r="O47" s="35"/>
+      <c r="N47" s="17"/>
+      <c r="O47" s="17"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
-      <c r="V47" s="2"/>
-      <c r="W47" s="2"/>
-      <c r="X47" s="2"/>
-      <c r="Y47" s="2"/>
-      <c r="Z47" s="2"/>
-      <c r="AA47" s="2"/>
-    </row>
-    <row r="48" spans="1:27" ht="12.75" customHeight="1">
+      <c r="V47" s="1"/>
+      <c r="W47" s="1"/>
+      <c r="X47" s="1"/>
+      <c r="Y47" s="1"/>
+      <c r="Z47" s="1"/>
+      <c r="AA47" s="1"/>
+    </row>
+    <row r="48" spans="1:27" ht="15.75">
       <c r="A48" s="37" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
-      <c r="B48" s="37"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="70"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="56"/>
-      <c r="H48" s="37"/>
-      <c r="I48" s="56"/>
-      <c r="J48" s="56"/>
-      <c r="K48" s="37"/>
-      <c r="L48" s="70"/>
-      <c r="M48" s="37"/>
-      <c r="N48" s="37"/>
-      <c r="O48" s="37"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="2"/>
-      <c r="R48" s="2"/>
-      <c r="S48" s="2"/>
-      <c r="T48" s="2"/>
-      <c r="U48" s="2"/>
-      <c r="V48" s="2"/>
-      <c r="W48" s="2"/>
-      <c r="X48" s="2"/>
-      <c r="Y48" s="2"/>
-      <c r="Z48" s="2"/>
-      <c r="AA48" s="2"/>
-    </row>
-    <row r="49" spans="1:27" ht="12.75" customHeight="1">
-      <c r="A49" s="38"/>
-      <c r="B49" s="38"/>
-      <c r="C49" s="55"/>
-      <c r="D49" s="69"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="55"/>
-      <c r="H49" s="38"/>
-      <c r="I49" s="55"/>
-      <c r="L49" s="69"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
-      <c r="R49" s="2"/>
-      <c r="S49" s="2"/>
-      <c r="T49" s="2"/>
-      <c r="U49" s="2"/>
-      <c r="V49" s="2"/>
-      <c r="W49" s="2"/>
-      <c r="X49" s="2"/>
-      <c r="Y49" s="2"/>
-      <c r="Z49" s="2"/>
-      <c r="AA49" s="2"/>
+      <c r="B48" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="68"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G48" s="54"/>
+      <c r="H48" s="35"/>
+      <c r="I48" s="54"/>
+      <c r="J48" s="54"/>
+      <c r="K48" s="35"/>
+      <c r="L48" s="68"/>
+      <c r="M48" s="35"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="3"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="3"/>
+      <c r="T48" s="3"/>
+      <c r="U48" s="3"/>
+      <c r="V48" s="3"/>
+      <c r="W48" s="3"/>
+      <c r="X48" s="3"/>
+      <c r="Y48" s="3"/>
+      <c r="Z48" s="3"/>
+      <c r="AA48" s="3"/>
+    </row>
+    <row r="49" spans="1:27" ht="26.25">
+      <c r="A49" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="C49" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="D49" s="68" t="s">
+        <v>150</v>
+      </c>
+      <c r="E49" s="35"/>
+      <c r="F49" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="G49" s="54"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="54"/>
+      <c r="J49" s="54"/>
+      <c r="K49" s="35"/>
+      <c r="L49" s="68"/>
+      <c r="M49" s="35"/>
+      <c r="N49" s="18"/>
+      <c r="O49" s="18"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="5"/>
+      <c r="R49" s="5"/>
+      <c r="S49" s="5"/>
+      <c r="T49" s="5"/>
+      <c r="U49" s="5"/>
+      <c r="V49" s="5"/>
+      <c r="W49" s="5"/>
+      <c r="X49" s="5"/>
+      <c r="Y49" s="5"/>
+      <c r="Z49" s="5"/>
+      <c r="AA49" s="5"/>
     </row>
     <row r="50" spans="1:27" ht="30.75">
       <c r="A50" s="37" t="s">
         <v>97</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C50" s="54" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D50" s="68"/>
       <c r="E50" s="35"/>
@@ -2973,96 +3023,80 @@
         <v>94</v>
       </c>
       <c r="I50" s="54" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
-      <c r="J50" s="54"/>
-      <c r="K50" s="54"/>
+      <c r="J50" s="54" t="s">
+        <v>140</v>
+      </c>
+      <c r="K50" s="35"/>
       <c r="L50" s="68"/>
-      <c r="M50" s="54"/>
-      <c r="N50" s="54"/>
-      <c r="O50" s="54"/>
-      <c r="P50" s="2"/>
-      <c r="Q50" s="2"/>
-      <c r="R50" s="2"/>
-      <c r="S50" s="2"/>
-      <c r="T50" s="2"/>
-      <c r="U50" s="2"/>
-      <c r="V50" s="2"/>
-      <c r="W50" s="2"/>
-      <c r="X50" s="2"/>
-      <c r="Y50" s="2"/>
-      <c r="Z50" s="2"/>
-      <c r="AA50" s="2"/>
+      <c r="M50" s="35"/>
+      <c r="N50" s="18"/>
+      <c r="O50" s="18"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="3"/>
+      <c r="T50" s="3"/>
+      <c r="U50" s="3"/>
+      <c r="V50" s="3"/>
+      <c r="W50" s="3"/>
+      <c r="X50" s="3"/>
+      <c r="Y50" s="3"/>
+      <c r="Z50" s="3"/>
+      <c r="AA50" s="3"/>
     </row>
     <row r="51" spans="1:27" ht="15.75">
-      <c r="A51" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="B51" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="C51" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="D51" s="68"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G51" s="54" t="s">
-        <v>147</v>
-      </c>
-      <c r="H51" s="35"/>
-      <c r="I51" s="54"/>
-      <c r="J51" s="54"/>
-      <c r="K51" s="54"/>
-      <c r="L51" s="68"/>
-      <c r="M51" s="54"/>
-      <c r="N51" s="54"/>
-      <c r="O51" s="54"/>
+      <c r="A51" s="38"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="58"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="38"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="55"/>
+      <c r="H51" s="38"/>
+      <c r="I51" s="55"/>
+      <c r="L51" s="69"/>
+      <c r="M51" s="38"/>
+      <c r="N51" s="38"/>
+      <c r="O51" s="38"/>
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
       <c r="S51" s="2"/>
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
-      <c r="V51" s="2"/>
-      <c r="W51" s="2"/>
-      <c r="X51" s="2"/>
-      <c r="Y51" s="2"/>
-      <c r="Z51" s="2"/>
-      <c r="AA51" s="2"/>
-    </row>
-    <row r="52" spans="1:27" ht="26.25">
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+      <c r="X51" s="1"/>
+      <c r="Y51" s="1"/>
+      <c r="Z51" s="1"/>
+      <c r="AA51" s="1"/>
+    </row>
+    <row r="52" spans="1:27" ht="15" customHeight="1">
       <c r="A52" s="37" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="B52" s="37" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
-      <c r="C52" s="54" t="s">
-        <v>143</v>
+      <c r="C52" s="56" t="s">
+        <v>148</v>
       </c>
-      <c r="D52" s="68" t="s">
-        <v>109</v>
+      <c r="D52" s="70"/>
+      <c r="E52" s="37" t="s">
+        <v>17</v>
       </c>
-      <c r="E52" s="35"/>
-      <c r="F52" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G52" s="54"/>
-      <c r="H52" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="I52" s="54" t="s">
-        <v>145</v>
-      </c>
-      <c r="J52" s="54"/>
-      <c r="K52" s="54"/>
-      <c r="L52" s="68"/>
-      <c r="M52" s="54"/>
-      <c r="N52" s="54"/>
-      <c r="O52" s="54"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="56"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="56"/>
+      <c r="J52" s="56"/>
+      <c r="K52" s="37"/>
+      <c r="L52" s="70"/>
+      <c r="M52" s="37"/>
+      <c r="N52" s="37"/>
+      <c r="O52" s="37"/>
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
@@ -3076,24 +3110,32 @@
       <c r="Z52" s="2"/>
       <c r="AA52" s="2"/>
     </row>
-    <row r="53" spans="1:27" ht="12.75" customHeight="1">
+    <row r="53" spans="1:27" ht="30.75">
       <c r="A53" s="37" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
-      <c r="B53" s="37"/>
-      <c r="C53" s="56"/>
-      <c r="D53" s="59"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="56"/>
-      <c r="H53" s="37"/>
-      <c r="I53" s="56"/>
-      <c r="J53" s="56"/>
-      <c r="K53" s="37"/>
-      <c r="L53" s="70"/>
-      <c r="M53" s="37"/>
-      <c r="N53" s="37"/>
-      <c r="O53" s="37"/>
+      <c r="B53" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="D53" s="68"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="54"/>
+      <c r="H53" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="I53" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="J53" s="54"/>
+      <c r="K53" s="35"/>
+      <c r="L53" s="68"/>
+      <c r="M53" s="35"/>
+      <c r="N53" s="35"/>
+      <c r="O53" s="35"/>
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
@@ -3107,22 +3149,32 @@
       <c r="Z53" s="2"/>
       <c r="AA53" s="2"/>
     </row>
-    <row r="54" spans="1:27" ht="12.75" customHeight="1">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="49"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="49"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="49"/>
-      <c r="J54" s="49"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="49"/>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2"/>
-      <c r="O54" s="2"/>
+    <row r="54" spans="1:27" ht="15.75">
+      <c r="A54" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="B54" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="D54" s="68"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="54"/>
+      <c r="H54" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="I54" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="J54" s="54"/>
+      <c r="K54" s="35"/>
+      <c r="L54" s="68"/>
+      <c r="M54" s="35"/>
+      <c r="N54" s="35"/>
+      <c r="O54" s="35"/>
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
@@ -3137,21 +3189,23 @@
       <c r="AA54" s="2"/>
     </row>
     <row r="55" spans="1:27" ht="12.75" customHeight="1">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="49"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="49"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="49"/>
-      <c r="J55" s="49"/>
-      <c r="K55" s="2"/>
-      <c r="L55" s="49"/>
-      <c r="M55" s="2"/>
-      <c r="N55" s="2"/>
-      <c r="O55" s="2"/>
+      <c r="A55" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55" s="37"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="70"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="56"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="56"/>
+      <c r="J55" s="56"/>
+      <c r="K55" s="37"/>
+      <c r="L55" s="70"/>
+      <c r="M55" s="37"/>
+      <c r="N55" s="37"/>
+      <c r="O55" s="37"/>
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
@@ -3166,18 +3220,16 @@
       <c r="AA55" s="2"/>
     </row>
     <row r="56" spans="1:27" ht="12.75" customHeight="1">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="49"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="49"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="49"/>
-      <c r="J56" s="49"/>
-      <c r="K56" s="2"/>
-      <c r="L56" s="49"/>
+      <c r="A56" s="38"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="55"/>
+      <c r="D56" s="69"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="55"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="55"/>
+      <c r="L56" s="69"/>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -3194,22 +3246,34 @@
       <c r="Z56" s="2"/>
       <c r="AA56" s="2"/>
     </row>
-    <row r="57" spans="1:27" ht="12.75" customHeight="1">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="49"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="49"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="49"/>
-      <c r="J57" s="49"/>
-      <c r="K57" s="2"/>
-      <c r="L57" s="49"/>
-      <c r="M57" s="2"/>
-      <c r="N57" s="2"/>
-      <c r="O57" s="2"/>
+    <row r="57" spans="1:27" ht="30.75">
+      <c r="A57" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="D57" s="68"/>
+      <c r="E57" s="35"/>
+      <c r="F57" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G57" s="54"/>
+      <c r="H57" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="I57" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="J57" s="54"/>
+      <c r="K57" s="54"/>
+      <c r="L57" s="68"/>
+      <c r="M57" s="54"/>
+      <c r="N57" s="54"/>
+      <c r="O57" s="54"/>
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
@@ -3223,22 +3287,32 @@
       <c r="Z57" s="2"/>
       <c r="AA57" s="2"/>
     </row>
-    <row r="58" spans="1:27" ht="12.75" customHeight="1">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="49"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="49"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="49"/>
-      <c r="J58" s="49"/>
-      <c r="K58" s="2"/>
-      <c r="L58" s="49"/>
-      <c r="M58" s="2"/>
-      <c r="N58" s="2"/>
-      <c r="O58" s="2"/>
+    <row r="58" spans="1:27" ht="15.75">
+      <c r="A58" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B58" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="C58" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="D58" s="68"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G58" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="H58" s="35"/>
+      <c r="I58" s="54"/>
+      <c r="J58" s="54"/>
+      <c r="K58" s="54"/>
+      <c r="L58" s="68"/>
+      <c r="M58" s="54"/>
+      <c r="N58" s="54"/>
+      <c r="O58" s="54"/>
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
@@ -3252,22 +3326,36 @@
       <c r="Z58" s="2"/>
       <c r="AA58" s="2"/>
     </row>
-    <row r="59" spans="1:27" ht="12.75" customHeight="1">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="49"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="49"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="49"/>
-      <c r="J59" s="49"/>
-      <c r="K59" s="2"/>
-      <c r="L59" s="49"/>
-      <c r="M59" s="2"/>
-      <c r="N59" s="2"/>
-      <c r="O59" s="2"/>
+    <row r="59" spans="1:27" ht="26.25">
+      <c r="A59" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="54" t="s">
+        <v>143</v>
+      </c>
+      <c r="D59" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="E59" s="35"/>
+      <c r="F59" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G59" s="54"/>
+      <c r="H59" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="I59" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="J59" s="54"/>
+      <c r="K59" s="54"/>
+      <c r="L59" s="68"/>
+      <c r="M59" s="54"/>
+      <c r="N59" s="54"/>
+      <c r="O59" s="54"/>
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
@@ -3282,21 +3370,23 @@
       <c r="AA59" s="2"/>
     </row>
     <row r="60" spans="1:27" ht="12.75" customHeight="1">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="49"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="49"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="49"/>
-      <c r="J60" s="49"/>
-      <c r="K60" s="2"/>
-      <c r="L60" s="49"/>
-      <c r="M60" s="2"/>
-      <c r="N60" s="2"/>
-      <c r="O60" s="2"/>
+      <c r="A60" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" s="37"/>
+      <c r="C60" s="56"/>
+      <c r="D60" s="59"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="56"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="56"/>
+      <c r="J60" s="56"/>
+      <c r="K60" s="37"/>
+      <c r="L60" s="70"/>
+      <c r="M60" s="37"/>
+      <c r="N60" s="37"/>
+      <c r="O60" s="37"/>
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
@@ -8298,7 +8388,7 @@
       <c r="Z232" s="2"/>
       <c r="AA232" s="2"/>
     </row>
-    <row r="233" spans="1:27" ht="15.75" customHeight="1">
+    <row r="233" spans="1:27" ht="12.75" customHeight="1">
       <c r="A233" s="2"/>
       <c r="B233" s="2"/>
       <c r="C233" s="49"/>
@@ -8327,7 +8417,7 @@
       <c r="Z233" s="2"/>
       <c r="AA233" s="2"/>
     </row>
-    <row r="234" spans="1:27" ht="15.75" customHeight="1">
+    <row r="234" spans="1:27" ht="12.75" customHeight="1">
       <c r="A234" s="2"/>
       <c r="B234" s="2"/>
       <c r="C234" s="49"/>
@@ -8356,7 +8446,7 @@
       <c r="Z234" s="2"/>
       <c r="AA234" s="2"/>
     </row>
-    <row r="235" spans="1:27" ht="15.75" customHeight="1">
+    <row r="235" spans="1:27" ht="12.75" customHeight="1">
       <c r="A235" s="2"/>
       <c r="B235" s="2"/>
       <c r="C235" s="49"/>
@@ -8385,7 +8475,7 @@
       <c r="Z235" s="2"/>
       <c r="AA235" s="2"/>
     </row>
-    <row r="236" spans="1:27" ht="15.75" customHeight="1">
+    <row r="236" spans="1:27" ht="12.75" customHeight="1">
       <c r="A236" s="2"/>
       <c r="B236" s="2"/>
       <c r="C236" s="49"/>
@@ -8414,7 +8504,7 @@
       <c r="Z236" s="2"/>
       <c r="AA236" s="2"/>
     </row>
-    <row r="237" spans="1:27" ht="15.75" customHeight="1">
+    <row r="237" spans="1:27" ht="12.75" customHeight="1">
       <c r="A237" s="2"/>
       <c r="B237" s="2"/>
       <c r="C237" s="49"/>
@@ -8443,7 +8533,7 @@
       <c r="Z237" s="2"/>
       <c r="AA237" s="2"/>
     </row>
-    <row r="238" spans="1:27" ht="15.75" customHeight="1">
+    <row r="238" spans="1:27" ht="12.75" customHeight="1">
       <c r="A238" s="2"/>
       <c r="B238" s="2"/>
       <c r="C238" s="49"/>
@@ -8472,7 +8562,7 @@
       <c r="Z238" s="2"/>
       <c r="AA238" s="2"/>
     </row>
-    <row r="239" spans="1:27" ht="15.75" customHeight="1">
+    <row r="239" spans="1:27" ht="12.75" customHeight="1">
       <c r="A239" s="2"/>
       <c r="B239" s="2"/>
       <c r="C239" s="49"/>
@@ -30773,7 +30863,7 @@
       <c r="Z1007" s="2"/>
       <c r="AA1007" s="2"/>
     </row>
-    <row r="1008" spans="1:27" ht="15" customHeight="1">
+    <row r="1008" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1008" s="2"/>
       <c r="B1008" s="2"/>
       <c r="C1008" s="49"/>
@@ -30786,8 +30876,23 @@
       <c r="J1008" s="49"/>
       <c r="K1008" s="2"/>
       <c r="L1008" s="49"/>
-    </row>
-    <row r="1009" spans="1:12" ht="15" customHeight="1">
+      <c r="M1008" s="2"/>
+      <c r="N1008" s="2"/>
+      <c r="O1008" s="2"/>
+      <c r="P1008" s="2"/>
+      <c r="Q1008" s="2"/>
+      <c r="R1008" s="2"/>
+      <c r="S1008" s="2"/>
+      <c r="T1008" s="2"/>
+      <c r="U1008" s="2"/>
+      <c r="V1008" s="2"/>
+      <c r="W1008" s="2"/>
+      <c r="X1008" s="2"/>
+      <c r="Y1008" s="2"/>
+      <c r="Z1008" s="2"/>
+      <c r="AA1008" s="2"/>
+    </row>
+    <row r="1009" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1009" s="2"/>
       <c r="B1009" s="2"/>
       <c r="C1009" s="49"/>
@@ -30800,8 +30905,23 @@
       <c r="J1009" s="49"/>
       <c r="K1009" s="2"/>
       <c r="L1009" s="49"/>
-    </row>
-    <row r="1010" spans="1:12" ht="15" customHeight="1">
+      <c r="M1009" s="2"/>
+      <c r="N1009" s="2"/>
+      <c r="O1009" s="2"/>
+      <c r="P1009" s="2"/>
+      <c r="Q1009" s="2"/>
+      <c r="R1009" s="2"/>
+      <c r="S1009" s="2"/>
+      <c r="T1009" s="2"/>
+      <c r="U1009" s="2"/>
+      <c r="V1009" s="2"/>
+      <c r="W1009" s="2"/>
+      <c r="X1009" s="2"/>
+      <c r="Y1009" s="2"/>
+      <c r="Z1009" s="2"/>
+      <c r="AA1009" s="2"/>
+    </row>
+    <row r="1010" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1010" s="2"/>
       <c r="B1010" s="2"/>
       <c r="C1010" s="49"/>
@@ -30814,8 +30934,23 @@
       <c r="J1010" s="49"/>
       <c r="K1010" s="2"/>
       <c r="L1010" s="49"/>
-    </row>
-    <row r="1011" spans="1:12" ht="15" customHeight="1">
+      <c r="M1010" s="2"/>
+      <c r="N1010" s="2"/>
+      <c r="O1010" s="2"/>
+      <c r="P1010" s="2"/>
+      <c r="Q1010" s="2"/>
+      <c r="R1010" s="2"/>
+      <c r="S1010" s="2"/>
+      <c r="T1010" s="2"/>
+      <c r="U1010" s="2"/>
+      <c r="V1010" s="2"/>
+      <c r="W1010" s="2"/>
+      <c r="X1010" s="2"/>
+      <c r="Y1010" s="2"/>
+      <c r="Z1010" s="2"/>
+      <c r="AA1010" s="2"/>
+    </row>
+    <row r="1011" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1011" s="2"/>
       <c r="B1011" s="2"/>
       <c r="C1011" s="49"/>
@@ -30828,8 +30963,23 @@
       <c r="J1011" s="49"/>
       <c r="K1011" s="2"/>
       <c r="L1011" s="49"/>
-    </row>
-    <row r="1012" spans="1:12" ht="15" customHeight="1">
+      <c r="M1011" s="2"/>
+      <c r="N1011" s="2"/>
+      <c r="O1011" s="2"/>
+      <c r="P1011" s="2"/>
+      <c r="Q1011" s="2"/>
+      <c r="R1011" s="2"/>
+      <c r="S1011" s="2"/>
+      <c r="T1011" s="2"/>
+      <c r="U1011" s="2"/>
+      <c r="V1011" s="2"/>
+      <c r="W1011" s="2"/>
+      <c r="X1011" s="2"/>
+      <c r="Y1011" s="2"/>
+      <c r="Z1011" s="2"/>
+      <c r="AA1011" s="2"/>
+    </row>
+    <row r="1012" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1012" s="2"/>
       <c r="B1012" s="2"/>
       <c r="C1012" s="49"/>
@@ -30842,8 +30992,23 @@
       <c r="J1012" s="49"/>
       <c r="K1012" s="2"/>
       <c r="L1012" s="49"/>
-    </row>
-    <row r="1013" spans="1:12" ht="15" customHeight="1">
+      <c r="M1012" s="2"/>
+      <c r="N1012" s="2"/>
+      <c r="O1012" s="2"/>
+      <c r="P1012" s="2"/>
+      <c r="Q1012" s="2"/>
+      <c r="R1012" s="2"/>
+      <c r="S1012" s="2"/>
+      <c r="T1012" s="2"/>
+      <c r="U1012" s="2"/>
+      <c r="V1012" s="2"/>
+      <c r="W1012" s="2"/>
+      <c r="X1012" s="2"/>
+      <c r="Y1012" s="2"/>
+      <c r="Z1012" s="2"/>
+      <c r="AA1012" s="2"/>
+    </row>
+    <row r="1013" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1013" s="2"/>
       <c r="B1013" s="2"/>
       <c r="C1013" s="49"/>
@@ -30856,8 +31021,23 @@
       <c r="J1013" s="49"/>
       <c r="K1013" s="2"/>
       <c r="L1013" s="49"/>
-    </row>
-    <row r="1014" spans="1:12" ht="15" customHeight="1">
+      <c r="M1013" s="2"/>
+      <c r="N1013" s="2"/>
+      <c r="O1013" s="2"/>
+      <c r="P1013" s="2"/>
+      <c r="Q1013" s="2"/>
+      <c r="R1013" s="2"/>
+      <c r="S1013" s="2"/>
+      <c r="T1013" s="2"/>
+      <c r="U1013" s="2"/>
+      <c r="V1013" s="2"/>
+      <c r="W1013" s="2"/>
+      <c r="X1013" s="2"/>
+      <c r="Y1013" s="2"/>
+      <c r="Z1013" s="2"/>
+      <c r="AA1013" s="2"/>
+    </row>
+    <row r="1014" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1014" s="2"/>
       <c r="B1014" s="2"/>
       <c r="C1014" s="49"/>
@@ -30870,8 +31050,23 @@
       <c r="J1014" s="49"/>
       <c r="K1014" s="2"/>
       <c r="L1014" s="49"/>
-    </row>
-    <row r="1015" spans="1:12" ht="15" customHeight="1">
+      <c r="M1014" s="2"/>
+      <c r="N1014" s="2"/>
+      <c r="O1014" s="2"/>
+      <c r="P1014" s="2"/>
+      <c r="Q1014" s="2"/>
+      <c r="R1014" s="2"/>
+      <c r="S1014" s="2"/>
+      <c r="T1014" s="2"/>
+      <c r="U1014" s="2"/>
+      <c r="V1014" s="2"/>
+      <c r="W1014" s="2"/>
+      <c r="X1014" s="2"/>
+      <c r="Y1014" s="2"/>
+      <c r="Z1014" s="2"/>
+      <c r="AA1014" s="2"/>
+    </row>
+    <row r="1015" spans="1:27" ht="15" customHeight="1">
       <c r="A1015" s="2"/>
       <c r="B1015" s="2"/>
       <c r="C1015" s="49"/>
@@ -30885,7 +31080,7 @@
       <c r="K1015" s="2"/>
       <c r="L1015" s="49"/>
     </row>
-    <row r="1016" spans="1:12" ht="15" customHeight="1">
+    <row r="1016" spans="1:27" ht="15" customHeight="1">
       <c r="A1016" s="2"/>
       <c r="B1016" s="2"/>
       <c r="C1016" s="49"/>
@@ -30899,7 +31094,7 @@
       <c r="K1016" s="2"/>
       <c r="L1016" s="49"/>
     </row>
-    <row r="1017" spans="1:12" ht="15" customHeight="1">
+    <row r="1017" spans="1:27" ht="15" customHeight="1">
       <c r="A1017" s="2"/>
       <c r="B1017" s="2"/>
       <c r="C1017" s="49"/>
@@ -30913,7 +31108,7 @@
       <c r="K1017" s="2"/>
       <c r="L1017" s="49"/>
     </row>
-    <row r="1018" spans="1:12" ht="15" customHeight="1">
+    <row r="1018" spans="1:27" ht="15" customHeight="1">
       <c r="A1018" s="2"/>
       <c r="B1018" s="2"/>
       <c r="C1018" s="49"/>
@@ -30927,7 +31122,7 @@
       <c r="K1018" s="2"/>
       <c r="L1018" s="49"/>
     </row>
-    <row r="1019" spans="1:12" ht="15" customHeight="1">
+    <row r="1019" spans="1:27" ht="15" customHeight="1">
       <c r="A1019" s="2"/>
       <c r="B1019" s="2"/>
       <c r="C1019" s="49"/>
@@ -30941,7 +31136,7 @@
       <c r="K1019" s="2"/>
       <c r="L1019" s="49"/>
     </row>
-    <row r="1020" spans="1:12" ht="15" customHeight="1">
+    <row r="1020" spans="1:27" ht="15" customHeight="1">
       <c r="A1020" s="2"/>
       <c r="B1020" s="2"/>
       <c r="C1020" s="49"/>
@@ -30955,7 +31150,7 @@
       <c r="K1020" s="2"/>
       <c r="L1020" s="49"/>
     </row>
-    <row r="1021" spans="1:12" ht="15" customHeight="1">
+    <row r="1021" spans="1:27" ht="15" customHeight="1">
       <c r="A1021" s="2"/>
       <c r="B1021" s="2"/>
       <c r="C1021" s="49"/>
@@ -30969,7 +31164,7 @@
       <c r="K1021" s="2"/>
       <c r="L1021" s="49"/>
     </row>
-    <row r="1022" spans="1:12" ht="15" customHeight="1">
+    <row r="1022" spans="1:27" ht="15" customHeight="1">
       <c r="A1022" s="2"/>
       <c r="B1022" s="2"/>
       <c r="C1022" s="49"/>
@@ -30983,7 +31178,7 @@
       <c r="K1022" s="2"/>
       <c r="L1022" s="49"/>
     </row>
-    <row r="1023" spans="1:12" ht="15" customHeight="1">
+    <row r="1023" spans="1:27" ht="15" customHeight="1">
       <c r="A1023" s="2"/>
       <c r="B1023" s="2"/>
       <c r="C1023" s="49"/>
@@ -30997,7 +31192,7 @@
       <c r="K1023" s="2"/>
       <c r="L1023" s="49"/>
     </row>
-    <row r="1024" spans="1:12" ht="15" customHeight="1">
+    <row r="1024" spans="1:27" ht="15" customHeight="1">
       <c r="A1024" s="2"/>
       <c r="B1024" s="2"/>
       <c r="C1024" s="49"/>
@@ -31010,6 +31205,104 @@
       <c r="J1024" s="49"/>
       <c r="K1024" s="2"/>
       <c r="L1024" s="49"/>
+    </row>
+    <row r="1025" spans="1:12" ht="15" customHeight="1">
+      <c r="A1025" s="2"/>
+      <c r="B1025" s="2"/>
+      <c r="C1025" s="49"/>
+      <c r="D1025" s="2"/>
+      <c r="E1025" s="2"/>
+      <c r="F1025" s="2"/>
+      <c r="G1025" s="49"/>
+      <c r="H1025" s="2"/>
+      <c r="I1025" s="49"/>
+      <c r="J1025" s="49"/>
+      <c r="K1025" s="2"/>
+      <c r="L1025" s="49"/>
+    </row>
+    <row r="1026" spans="1:12" ht="15" customHeight="1">
+      <c r="A1026" s="2"/>
+      <c r="B1026" s="2"/>
+      <c r="C1026" s="49"/>
+      <c r="D1026" s="2"/>
+      <c r="E1026" s="2"/>
+      <c r="F1026" s="2"/>
+      <c r="G1026" s="49"/>
+      <c r="H1026" s="2"/>
+      <c r="I1026" s="49"/>
+      <c r="J1026" s="49"/>
+      <c r="K1026" s="2"/>
+      <c r="L1026" s="49"/>
+    </row>
+    <row r="1027" spans="1:12" ht="15" customHeight="1">
+      <c r="A1027" s="2"/>
+      <c r="B1027" s="2"/>
+      <c r="C1027" s="49"/>
+      <c r="D1027" s="2"/>
+      <c r="E1027" s="2"/>
+      <c r="F1027" s="2"/>
+      <c r="G1027" s="49"/>
+      <c r="H1027" s="2"/>
+      <c r="I1027" s="49"/>
+      <c r="J1027" s="49"/>
+      <c r="K1027" s="2"/>
+      <c r="L1027" s="49"/>
+    </row>
+    <row r="1028" spans="1:12" ht="15" customHeight="1">
+      <c r="A1028" s="2"/>
+      <c r="B1028" s="2"/>
+      <c r="C1028" s="49"/>
+      <c r="D1028" s="2"/>
+      <c r="E1028" s="2"/>
+      <c r="F1028" s="2"/>
+      <c r="G1028" s="49"/>
+      <c r="H1028" s="2"/>
+      <c r="I1028" s="49"/>
+      <c r="J1028" s="49"/>
+      <c r="K1028" s="2"/>
+      <c r="L1028" s="49"/>
+    </row>
+    <row r="1029" spans="1:12" ht="15" customHeight="1">
+      <c r="A1029" s="2"/>
+      <c r="B1029" s="2"/>
+      <c r="C1029" s="49"/>
+      <c r="D1029" s="2"/>
+      <c r="E1029" s="2"/>
+      <c r="F1029" s="2"/>
+      <c r="G1029" s="49"/>
+      <c r="H1029" s="2"/>
+      <c r="I1029" s="49"/>
+      <c r="J1029" s="49"/>
+      <c r="K1029" s="2"/>
+      <c r="L1029" s="49"/>
+    </row>
+    <row r="1030" spans="1:12" ht="15" customHeight="1">
+      <c r="A1030" s="2"/>
+      <c r="B1030" s="2"/>
+      <c r="C1030" s="49"/>
+      <c r="D1030" s="2"/>
+      <c r="E1030" s="2"/>
+      <c r="F1030" s="2"/>
+      <c r="G1030" s="49"/>
+      <c r="H1030" s="2"/>
+      <c r="I1030" s="49"/>
+      <c r="J1030" s="49"/>
+      <c r="K1030" s="2"/>
+      <c r="L1030" s="49"/>
+    </row>
+    <row r="1031" spans="1:12" ht="15" customHeight="1">
+      <c r="A1031" s="2"/>
+      <c r="B1031" s="2"/>
+      <c r="C1031" s="49"/>
+      <c r="D1031" s="2"/>
+      <c r="E1031" s="2"/>
+      <c r="F1031" s="2"/>
+      <c r="G1031" s="49"/>
+      <c r="H1031" s="2"/>
+      <c r="I1031" s="49"/>
+      <c r="J1031" s="49"/>
+      <c r="K1031" s="2"/>
+      <c r="L1031" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>

</xml_diff>

<commit_message>
Added label to a group #108
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/enroll.xlsx
+++ b/config/itech-aurum/forms/app/enroll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-108\itech-aurum\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9806D289-A2CB-4589-BABF-6C0E41F022BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D30E5B-FE3D-4D5B-8A5B-C6EF07AEB2D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="178">
   <si>
     <t>type</t>
   </si>
@@ -1175,10 +1175,10 @@
   <dimension ref="A1:AA1031"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P27" sqref="P27"/>
+      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -2077,7 +2077,9 @@
       <c r="B25" s="77" t="s">
         <v>172</v>
       </c>
-      <c r="C25" s="78"/>
+      <c r="C25" s="78" t="s">
+        <v>40</v>
+      </c>
       <c r="D25" s="79" t="s">
         <v>173</v>
       </c>

</xml_diff>

<commit_message>
feat: improve reports data structure and clean ui fields
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/enroll.xlsx
+++ b/config/itech-aurum/forms/app/enroll.xlsx
@@ -3045,7 +3045,9 @@
       </c>
       <c r="M23" s="41"/>
       <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
+      <c r="O23" t="s" s="42">
+        <v>23</v>
+      </c>
       <c r="P23" s="14"/>
       <c r="Q23" s="15"/>
       <c r="R23" s="15"/>
@@ -3080,7 +3082,9 @@
       </c>
       <c r="M24" s="41"/>
       <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
+      <c r="O24" t="s" s="42">
+        <v>23</v>
+      </c>
       <c r="P24" s="14"/>
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>

</xml_diff>

<commit_message>
feat: add alt phone to report
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/enroll.xlsx
+++ b/config/itech-aurum/forms/app/enroll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54B42F1-E3FA-334C-9E77-26F1EA1F59EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC6B636-0661-B049-A5F9-0ACB496F4E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="155">
   <si>
     <t>type</t>
   </si>
@@ -211,9 +211,6 @@
   </si>
   <si>
     <t>number</t>
-  </si>
-  <si>
-    <t>regex(., '^[0-9]{5,9}$')</t>
   </si>
   <si>
     <t>Please enter between 5 - 9 digits</t>
@@ -466,9 +463,6 @@
     <t>Name of the person filling the form must be supplied</t>
   </si>
   <si>
-    <t>Africaans</t>
-  </si>
-  <si>
     <t>s_enrolled_by</t>
   </si>
   <si>
@@ -484,7 +478,16 @@
     <t>&lt;b&gt;Enrolled by&lt;/b&gt;: ${enrolled_by}</t>
   </si>
   <si>
-    <t>africaans</t>
+    <t>r_alternative_phone</t>
+  </si>
+  <si>
+    <t>../person/alternative_phone</t>
+  </si>
+  <si>
+    <t>afrikaans</t>
+  </si>
+  <si>
+    <t>Afrikaans</t>
   </si>
 </sst>
 </file>
@@ -1989,10 +1992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1024"/>
+  <dimension ref="A1:Z1025"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView showGridLines="0" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2057,7 +2060,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
@@ -2299,7 +2302,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>37</v>
@@ -2521,7 +2524,7 @@
         <v>42</v>
       </c>
       <c r="B15" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C15" s="51" t="s">
         <v>35</v>
@@ -2597,7 +2600,7 @@
         <v>42</v>
       </c>
       <c r="B17" s="48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C17" s="51" t="s">
         <v>40</v>
@@ -2610,7 +2613,7 @@
       <c r="I17" s="46"/>
       <c r="J17" s="46"/>
       <c r="K17" s="45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L17" s="46"/>
       <c r="M17" s="46"/>
@@ -2633,7 +2636,7 @@
         <v>42</v>
       </c>
       <c r="B18" s="48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C18" s="51" t="s">
         <v>47</v>
@@ -2669,7 +2672,7 @@
         <v>42</v>
       </c>
       <c r="B19" s="48" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="C19" s="51" t="s">
         <v>40</v>
@@ -2682,7 +2685,7 @@
       <c r="I19" s="46"/>
       <c r="J19" s="46"/>
       <c r="K19" s="45" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="L19" s="46"/>
       <c r="M19" s="46"/>
@@ -2705,7 +2708,7 @@
         <v>42</v>
       </c>
       <c r="B20" s="48" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C20" s="51" t="s">
         <v>40</v>
@@ -2718,7 +2721,7 @@
       <c r="I20" s="46"/>
       <c r="J20" s="46"/>
       <c r="K20" s="45" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="L20" s="46"/>
       <c r="M20" s="46"/>
@@ -2737,24 +2740,24 @@
       <c r="Z20" s="46"/>
     </row>
     <row r="21" spans="1:26" s="47" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="59" t="s">
+      <c r="A21" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="60" t="s">
-        <v>149</v>
+      <c r="B21" s="48" t="s">
+        <v>131</v>
       </c>
-      <c r="C21" s="61" t="s">
+      <c r="C21" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
       <c r="F21" s="46"/>
       <c r="G21" s="46"/>
       <c r="H21" s="46"/>
       <c r="I21" s="46"/>
       <c r="J21" s="46"/>
       <c r="K21" s="45" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="L21" s="46"/>
       <c r="M21" s="46"/>
@@ -2773,24 +2776,24 @@
       <c r="Z21" s="46"/>
     </row>
     <row r="22" spans="1:26" s="47" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="48" t="s">
-        <v>119</v>
+      <c r="B22" s="60" t="s">
+        <v>147</v>
       </c>
-      <c r="C22" s="51" t="s">
-        <v>50</v>
+      <c r="C22" s="61" t="s">
+        <v>40</v>
       </c>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
       <c r="F22" s="46"/>
       <c r="G22" s="46"/>
       <c r="H22" s="46"/>
       <c r="I22" s="46"/>
       <c r="J22" s="46"/>
       <c r="K22" s="45" t="s">
-        <v>51</v>
+        <v>148</v>
       </c>
       <c r="L22" s="46"/>
       <c r="M22" s="46"/>
@@ -2809,24 +2812,24 @@
       <c r="Z22" s="46"/>
     </row>
     <row r="23" spans="1:26" s="47" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="59" t="s">
+      <c r="A23" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="60" t="s">
-        <v>138</v>
+      <c r="B23" s="48" t="s">
+        <v>118</v>
       </c>
-      <c r="C23" s="61" t="s">
-        <v>40</v>
+      <c r="C23" s="51" t="s">
+        <v>50</v>
       </c>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
       <c r="F23" s="46"/>
       <c r="G23" s="46"/>
       <c r="H23" s="46"/>
       <c r="I23" s="46"/>
       <c r="J23" s="46"/>
       <c r="K23" s="45" t="s">
-        <v>139</v>
+        <v>51</v>
       </c>
       <c r="L23" s="46"/>
       <c r="M23" s="46"/>
@@ -2844,129 +2847,123 @@
       <c r="Y23" s="46"/>
       <c r="Z23" s="46"/>
     </row>
-    <row r="24" spans="1:26" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
+    <row r="24" spans="1:26" s="47" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="46"/>
+      <c r="Q24" s="46"/>
+      <c r="R24" s="46"/>
+      <c r="S24" s="46"/>
+      <c r="T24" s="46"/>
+      <c r="U24" s="46"/>
+      <c r="V24" s="46"/>
+      <c r="W24" s="46"/>
+      <c r="X24" s="46"/>
+      <c r="Y24" s="46"/>
+      <c r="Z24" s="46"/>
+    </row>
+    <row r="25" spans="1:26" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="26"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="C24" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27" t="s">
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="27"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="27"/>
-      <c r="T24" s="27"/>
-      <c r="U24" s="27"/>
-      <c r="V24" s="27"/>
-      <c r="W24" s="27"/>
-      <c r="X24" s="27"/>
-      <c r="Y24" s="27"/>
-      <c r="Z24" s="27" t="s">
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="27"/>
+      <c r="R25" s="27"/>
+      <c r="S25" s="27"/>
+      <c r="T25" s="27"/>
+      <c r="U25" s="27"/>
+      <c r="V25" s="27"/>
+      <c r="W25" s="27"/>
+      <c r="X25" s="27"/>
+      <c r="Y25" s="27"/>
+      <c r="Z25" s="27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-      <c r="S25" s="6"/>
-      <c r="T25" s="6"/>
-      <c r="U25" s="6"/>
-      <c r="V25" s="6"/>
-      <c r="W25" s="6"/>
-      <c r="X25" s="6"/>
-      <c r="Y25" s="6"/>
-      <c r="Z25" s="6"/>
-    </row>
-    <row r="26" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="30"/>
-      <c r="E26" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="M26" s="30"/>
-      <c r="N26" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="O26" s="30"/>
-      <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
-      <c r="S26" s="30"/>
-      <c r="T26" s="30"/>
-      <c r="U26" s="30"/>
-      <c r="V26" s="30"/>
-      <c r="W26" s="30"/>
-      <c r="X26" s="30"/>
-      <c r="Y26" s="30"/>
-      <c r="Z26" s="30" t="s">
-        <v>21</v>
-      </c>
+    <row r="26" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="6"/>
+      <c r="X26" s="6"/>
+      <c r="Y26" s="6"/>
+      <c r="Z26" s="6"/>
     </row>
     <row r="27" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="38" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C27" s="52" t="s">
         <v>40</v>
       </c>
       <c r="D27" s="30"/>
       <c r="E27" s="29" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F27" s="30"/>
       <c r="G27" s="30"/>
@@ -2974,9 +2971,13 @@
       <c r="I27" s="30"/>
       <c r="J27" s="30"/>
       <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
+      <c r="L27" s="29" t="s">
+        <v>52</v>
+      </c>
       <c r="M27" s="30"/>
-      <c r="N27" s="30"/>
+      <c r="N27" s="30" t="s">
+        <v>21</v>
+      </c>
       <c r="O27" s="30"/>
       <c r="P27" s="30"/>
       <c r="Q27" s="30"/>
@@ -2988,14 +2989,16 @@
       <c r="W27" s="30"/>
       <c r="X27" s="30"/>
       <c r="Y27" s="30"/>
-      <c r="Z27" s="30"/>
+      <c r="Z27" s="30" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="28" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="38" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B28" s="38" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C28" s="52" t="s">
         <v>40</v>
@@ -3009,9 +3012,7 @@
       <c r="H28" s="30"/>
       <c r="I28" s="30"/>
       <c r="J28" s="30"/>
-      <c r="K28" s="29" t="s">
-        <v>53</v>
-      </c>
+      <c r="K28" s="30"/>
       <c r="L28" s="30"/>
       <c r="M28" s="30"/>
       <c r="N28" s="30"/>
@@ -3030,24 +3031,26 @@
     </row>
     <row r="29" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="38" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B29" s="38" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C29" s="52" t="s">
         <v>40</v>
       </c>
       <c r="D29" s="30"/>
       <c r="E29" s="29" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F29" s="30"/>
       <c r="G29" s="30"/>
       <c r="H29" s="30"/>
       <c r="I29" s="30"/>
       <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
+      <c r="K29" s="29" t="s">
+        <v>53</v>
+      </c>
       <c r="L29" s="30"/>
       <c r="M29" s="30"/>
       <c r="N29" s="30"/>
@@ -3066,26 +3069,24 @@
     </row>
     <row r="30" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="38" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B30" s="38" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C30" s="52" t="s">
         <v>40</v>
       </c>
       <c r="D30" s="30"/>
       <c r="E30" s="29" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F30" s="30"/>
       <c r="G30" s="30"/>
       <c r="H30" s="30"/>
       <c r="I30" s="30"/>
       <c r="J30" s="30"/>
-      <c r="K30" s="29" t="s">
-        <v>54</v>
-      </c>
+      <c r="K30" s="30"/>
       <c r="L30" s="30"/>
       <c r="M30" s="30"/>
       <c r="N30" s="30"/>
@@ -3104,20 +3105,26 @@
     </row>
     <row r="31" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="38" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
-      <c r="B31" s="39"/>
+      <c r="B31" s="38" t="s">
+        <v>30</v>
+      </c>
       <c r="C31" s="52" t="s">
         <v>40</v>
       </c>
       <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
+      <c r="E31" s="29" t="s">
+        <v>21</v>
+      </c>
       <c r="F31" s="30"/>
       <c r="G31" s="30"/>
       <c r="H31" s="30"/>
       <c r="I31" s="30"/>
       <c r="J31" s="30"/>
-      <c r="K31" s="30"/>
+      <c r="K31" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="L31" s="30"/>
       <c r="M31" s="30"/>
       <c r="N31" s="30"/>
@@ -3168,26 +3175,20 @@
     </row>
     <row r="33" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
-      <c r="B33" s="38" t="s">
-        <v>0</v>
-      </c>
+      <c r="B33" s="39"/>
       <c r="C33" s="52" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="D33" s="30"/>
       <c r="E33" s="30"/>
       <c r="F33" s="30"/>
       <c r="G33" s="30"/>
-      <c r="H33" s="29" t="s">
-        <v>45</v>
-      </c>
+      <c r="H33" s="30"/>
       <c r="I33" s="30"/>
       <c r="J33" s="30"/>
-      <c r="K33" s="29" t="s">
-        <v>56</v>
-      </c>
+      <c r="K33" s="30"/>
       <c r="L33" s="30"/>
       <c r="M33" s="30"/>
       <c r="N33" s="30"/>
@@ -3204,30 +3205,28 @@
       <c r="Y33" s="30"/>
       <c r="Z33" s="30"/>
     </row>
-    <row r="34" spans="1:26" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="38" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B34" s="38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
-      <c r="C34" s="53" t="s">
-        <v>86</v>
+      <c r="C34" s="52" t="s">
+        <v>55</v>
       </c>
       <c r="D34" s="30"/>
       <c r="E34" s="30"/>
-      <c r="F34" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="G34" s="29" t="s">
-        <v>57</v>
-      </c>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
       <c r="H34" s="29" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="I34" s="30"/>
       <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
+      <c r="K34" s="29" t="s">
+        <v>56</v>
+      </c>
       <c r="L34" s="30"/>
       <c r="M34" s="30"/>
       <c r="N34" s="30"/>
@@ -3245,58 +3244,62 @@
       <c r="Z34" s="30"/>
     </row>
     <row r="35" spans="1:26" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="G35" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="H35" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="30"/>
+      <c r="L35" s="30"/>
+      <c r="M35" s="30"/>
+      <c r="N35" s="30"/>
+      <c r="O35" s="30"/>
+      <c r="P35" s="30"/>
+      <c r="Q35" s="30"/>
+      <c r="R35" s="30"/>
+      <c r="S35" s="30"/>
+      <c r="T35" s="30"/>
+      <c r="U35" s="30"/>
+      <c r="V35" s="30"/>
+      <c r="W35" s="30"/>
+      <c r="X35" s="30"/>
+      <c r="Y35" s="30"/>
+      <c r="Z35" s="30"/>
+    </row>
+    <row r="36" spans="1:26" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B36" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="52" t="s">
+      <c r="C36" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34" t="s">
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="34"/>
-      <c r="K35" s="34"/>
-      <c r="L35" s="34"/>
-      <c r="M35" s="34"/>
-      <c r="N35" s="34"/>
-      <c r="O35" s="34"/>
-      <c r="P35" s="34"/>
-      <c r="Q35" s="34"/>
-      <c r="R35" s="34"/>
-      <c r="S35" s="34"/>
-      <c r="T35" s="34"/>
-      <c r="U35" s="34"/>
-      <c r="V35" s="34"/>
-      <c r="W35" s="34"/>
-      <c r="X35" s="34"/>
-      <c r="Y35" s="34"/>
-      <c r="Z35" s="34"/>
-    </row>
-    <row r="36" spans="1:26" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="D36" s="34"/>
-      <c r="E36" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="F36" s="33"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
       <c r="I36" s="34"/>
       <c r="J36" s="34"/>
       <c r="K36" s="34"/>
@@ -3318,19 +3321,19 @@
     </row>
     <row r="37" spans="1:26" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="42" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="B37" s="42" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
-      <c r="C37" s="52" t="s">
-        <v>40</v>
+      <c r="C37" s="43" t="s">
+        <v>84</v>
       </c>
-      <c r="D37" s="35"/>
+      <c r="D37" s="34"/>
       <c r="E37" s="33" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
-      <c r="F37" s="34"/>
+      <c r="F37" s="33"/>
       <c r="G37" s="30"/>
       <c r="H37" s="30"/>
       <c r="I37" s="34"/>
@@ -3353,18 +3356,22 @@
       <c r="Z37" s="34"/>
     </row>
     <row r="38" spans="1:26" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="41" t="s">
-        <v>41</v>
+      <c r="A38" s="42" t="s">
+        <v>18</v>
       </c>
-      <c r="B38" s="44"/>
+      <c r="B38" s="42" t="s">
+        <v>1</v>
+      </c>
       <c r="C38" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="33" t="s">
+        <v>21</v>
+      </c>
       <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="34"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
       <c r="I38" s="34"/>
       <c r="J38" s="34"/>
       <c r="K38" s="34"/>
@@ -3385,64 +3392,56 @@
       <c r="Z38" s="34"/>
     </row>
     <row r="39" spans="1:26" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="38" t="s">
+      <c r="A39" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="44"/>
+      <c r="C39" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
+      <c r="K39" s="34"/>
+      <c r="L39" s="34"/>
+      <c r="M39" s="34"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="34"/>
+      <c r="P39" s="34"/>
+      <c r="Q39" s="34"/>
+      <c r="R39" s="34"/>
+      <c r="S39" s="34"/>
+      <c r="T39" s="34"/>
+      <c r="U39" s="34"/>
+      <c r="V39" s="34"/>
+      <c r="W39" s="34"/>
+      <c r="X39" s="34"/>
+      <c r="Y39" s="34"/>
+      <c r="Z39" s="34"/>
+    </row>
+    <row r="40" spans="1:26" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="38" t="s">
+      <c r="B40" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="52" t="s">
-        <v>145</v>
-      </c>
-      <c r="D39" s="30"/>
-      <c r="E39" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="F39" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="H39" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="30"/>
-      <c r="N39" s="30"/>
-      <c r="O39" s="30"/>
-      <c r="P39" s="30"/>
-      <c r="Q39" s="30"/>
-      <c r="R39" s="30"/>
-      <c r="S39" s="30"/>
-      <c r="T39" s="30"/>
-      <c r="U39" s="30"/>
-      <c r="V39" s="30"/>
-      <c r="W39" s="30"/>
-      <c r="X39" s="30"/>
-      <c r="Y39" s="30"/>
-      <c r="Z39" s="30"/>
-    </row>
-    <row r="40" spans="1:26" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="B40" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="C40" s="53" t="s">
-        <v>87</v>
+      <c r="C40" s="52" t="s">
+        <v>144</v>
       </c>
       <c r="D40" s="30"/>
       <c r="E40" s="29"/>
-      <c r="F40" s="32" t="s">
+      <c r="F40" s="29" t="s">
         <v>33</v>
       </c>
       <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
+      <c r="H40" s="29" t="s">
+        <v>63</v>
+      </c>
       <c r="I40" s="30"/>
       <c r="J40" s="30"/>
       <c r="K40" s="30"/>
@@ -3463,29 +3462,25 @@
       <c r="Z40" s="30"/>
     </row>
     <row r="41" spans="1:26" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="38" t="s">
-        <v>83</v>
+      <c r="A41" s="40" t="s">
+        <v>90</v>
       </c>
-      <c r="B41" s="38" t="s">
-        <v>84</v>
+      <c r="B41" s="40" t="s">
+        <v>91</v>
       </c>
       <c r="C41" s="53" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D41" s="30"/>
-      <c r="E41" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="F41" s="29" t="s">
+      <c r="E41" s="29"/>
+      <c r="F41" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="G41" s="32"/>
-      <c r="H41" s="29" t="s">
-        <v>65</v>
-      </c>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
       <c r="I41" s="30"/>
       <c r="J41" s="30"/>
-      <c r="K41" s="36"/>
+      <c r="K41" s="30"/>
       <c r="L41" s="30"/>
       <c r="M41" s="30"/>
       <c r="N41" s="30"/>
@@ -3502,32 +3497,30 @@
       <c r="Y41" s="30"/>
       <c r="Z41" s="30"/>
     </row>
-    <row r="42" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:26" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="38" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="C42" s="53" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
+      <c r="E42" s="29" t="s">
+        <v>62</v>
+      </c>
       <c r="F42" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="G42" s="29" t="s">
-        <v>102</v>
+      <c r="G42" s="32"/>
+      <c r="H42" s="29" t="s">
+        <v>64</v>
       </c>
-      <c r="H42" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="I42" s="37" t="s">
-        <v>103</v>
-      </c>
+      <c r="I42" s="30"/>
       <c r="J42" s="30"/>
-      <c r="K42" s="30"/>
+      <c r="K42" s="36"/>
       <c r="L42" s="30"/>
       <c r="M42" s="30"/>
       <c r="N42" s="30"/>
@@ -3544,29 +3537,29 @@
       <c r="Y42" s="30"/>
       <c r="Z42" s="30"/>
     </row>
-    <row r="43" spans="1:26" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="38" t="s">
         <v>18</v>
       </c>
       <c r="B43" s="38" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C43" s="53" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D43" s="30"/>
       <c r="E43" s="30"/>
       <c r="F43" s="29" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="G43" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H43" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I43" s="37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J43" s="30"/>
       <c r="K43" s="30"/>
@@ -3588,22 +3581,28 @@
     </row>
     <row r="44" spans="1:26" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="38" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
-      <c r="C44" s="52" t="s">
-        <v>70</v>
+      <c r="C44" s="53" t="s">
+        <v>89</v>
       </c>
       <c r="D44" s="30"/>
       <c r="E44" s="30"/>
       <c r="F44" s="29" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
-      <c r="G44" s="30"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
+      <c r="G44" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="H44" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="I44" s="37" t="s">
+        <v>102</v>
+      </c>
       <c r="J44" s="30"/>
       <c r="K44" s="30"/>
       <c r="L44" s="30"/>
@@ -3624,28 +3623,22 @@
     </row>
     <row r="45" spans="1:26" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="38" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="B45" s="38" t="s">
-        <v>142</v>
+        <v>49</v>
       </c>
       <c r="C45" s="52" t="s">
-        <v>143</v>
+        <v>69</v>
       </c>
       <c r="D45" s="30"/>
       <c r="E45" s="30"/>
       <c r="F45" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="G45" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="H45" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="I45" s="30" t="s">
-        <v>144</v>
-      </c>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="30"/>
       <c r="J45" s="30"/>
       <c r="K45" s="30"/>
       <c r="L45" s="30"/>
@@ -3669,17 +3662,25 @@
         <v>18</v>
       </c>
       <c r="B46" s="38" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="C46" s="52" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
       <c r="D46" s="30"/>
       <c r="E46" s="30"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="30"/>
-      <c r="H46" s="30"/>
-      <c r="I46" s="30"/>
+      <c r="F46" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="G46" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="H46" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="I46" s="30" t="s">
+        <v>143</v>
+      </c>
       <c r="J46" s="30"/>
       <c r="K46" s="30"/>
       <c r="L46" s="30"/>
@@ -3698,15 +3699,19 @@
       <c r="Y46" s="30"/>
       <c r="Z46" s="30"/>
     </row>
-    <row r="47" spans="1:26" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:26" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="38" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
-      <c r="B47" s="39"/>
-      <c r="C47" s="54"/>
+      <c r="B47" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="52" t="s">
+        <v>94</v>
+      </c>
       <c r="D47" s="30"/>
       <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
+      <c r="F47" s="29"/>
       <c r="G47" s="30"/>
       <c r="H47" s="30"/>
       <c r="I47" s="30"/>
@@ -3728,57 +3733,49 @@
       <c r="Y47" s="30"/>
       <c r="Z47" s="30"/>
     </row>
-    <row r="48" spans="1:26" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="27" t="s">
+    <row r="48" spans="1:26" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="39"/>
+      <c r="C48" s="54"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="30"/>
+      <c r="K48" s="30"/>
+      <c r="L48" s="30"/>
+      <c r="M48" s="30"/>
+      <c r="N48" s="30"/>
+      <c r="O48" s="30"/>
+      <c r="P48" s="30"/>
+      <c r="Q48" s="30"/>
+      <c r="R48" s="30"/>
+      <c r="S48" s="30"/>
+      <c r="T48" s="30"/>
+      <c r="U48" s="30"/>
+      <c r="V48" s="30"/>
+      <c r="W48" s="30"/>
+      <c r="X48" s="30"/>
+      <c r="Y48" s="30"/>
+      <c r="Z48" s="30"/>
+    </row>
+    <row r="49" spans="1:26" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B48" s="27" t="s">
+      <c r="B49" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="55" t="s">
-        <v>97</v>
-      </c>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
-      <c r="H48" s="27"/>
-      <c r="I48" s="27"/>
-      <c r="J48" s="27"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="27"/>
-      <c r="M48" s="27"/>
-      <c r="N48" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="O48" s="27"/>
-      <c r="P48" s="27"/>
-      <c r="Q48" s="27"/>
-      <c r="R48" s="27"/>
-      <c r="S48" s="27"/>
-      <c r="T48" s="27"/>
-      <c r="U48" s="27"/>
-      <c r="V48" s="27"/>
-      <c r="W48" s="27"/>
-      <c r="X48" s="27"/>
-      <c r="Y48" s="27"/>
-      <c r="Z48" s="27"/>
-    </row>
-    <row r="49" spans="1:26" s="28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="B49" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="C49" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D49" s="26"/>
-      <c r="E49" s="25" t="s">
-        <v>101</v>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27" t="s">
+        <v>109</v>
       </c>
       <c r="F49" s="27"/>
       <c r="G49" s="27"/>
@@ -3788,7 +3785,9 @@
       <c r="K49" s="27"/>
       <c r="L49" s="27"/>
       <c r="M49" s="27"/>
-      <c r="N49" s="27"/>
+      <c r="N49" s="27" t="s">
+        <v>21</v>
+      </c>
       <c r="O49" s="27"/>
       <c r="P49" s="27"/>
       <c r="Q49" s="27"/>
@@ -3802,18 +3801,20 @@
       <c r="Y49" s="27"/>
       <c r="Z49" s="27"/>
     </row>
-    <row r="50" spans="1:26" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26" s="28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="B50" s="23" t="s">
-        <v>104</v>
-      </c>
       <c r="C50" s="24" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D50" s="26"/>
-      <c r="E50" s="25"/>
+      <c r="E50" s="25" t="s">
+        <v>100</v>
+      </c>
       <c r="F50" s="27"/>
       <c r="G50" s="27"/>
       <c r="H50" s="27"/>
@@ -3838,18 +3839,16 @@
     </row>
     <row r="51" spans="1:26" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D51" s="26"/>
-      <c r="E51" s="25" t="s">
-        <v>107</v>
-      </c>
+      <c r="E51" s="25"/>
       <c r="F51" s="27"/>
       <c r="G51" s="27"/>
       <c r="H51" s="27"/>
@@ -3874,16 +3873,18 @@
     </row>
     <row r="52" spans="1:26" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="D52" s="26"/>
-      <c r="E52" s="25"/>
+      <c r="E52" s="25" t="s">
+        <v>106</v>
+      </c>
       <c r="F52" s="27"/>
       <c r="G52" s="27"/>
       <c r="H52" s="27"/>
@@ -3908,10 +3909,10 @@
     </row>
     <row r="53" spans="1:26" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C53" s="24" t="s">
         <v>136</v>
@@ -3942,13 +3943,13 @@
     </row>
     <row r="54" spans="1:26" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="D54" s="26"/>
       <c r="E54" s="25"/>
@@ -3976,13 +3977,13 @@
     </row>
     <row r="55" spans="1:26" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="D55" s="26"/>
       <c r="E55" s="25"/>
@@ -4010,13 +4011,13 @@
     </row>
     <row r="56" spans="1:26" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D56" s="26"/>
       <c r="E56" s="25"/>
@@ -4044,13 +4045,13 @@
     </row>
     <row r="57" spans="1:26" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="D57" s="26"/>
       <c r="E57" s="25"/>
@@ -4078,13 +4079,13 @@
     </row>
     <row r="58" spans="1:26" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D58" s="26"/>
       <c r="E58" s="25"/>
@@ -4112,13 +4113,13 @@
     </row>
     <row r="59" spans="1:26" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D59" s="26"/>
       <c r="E59" s="25"/>
@@ -4146,13 +4147,13 @@
     </row>
     <row r="60" spans="1:26" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="D60" s="26"/>
       <c r="E60" s="25"/>
@@ -4178,38 +4179,44 @@
       <c r="Y60" s="27"/>
       <c r="Z60" s="27"/>
     </row>
-    <row r="61" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="6" t="s">
+    <row r="61" spans="1:26" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D61" s="26"/>
+      <c r="E61" s="25"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="27"/>
+      <c r="I61" s="27"/>
+      <c r="J61" s="27"/>
+      <c r="K61" s="27"/>
+      <c r="L61" s="27"/>
+      <c r="M61" s="27"/>
+      <c r="N61" s="27"/>
+      <c r="O61" s="27"/>
+      <c r="P61" s="27"/>
+      <c r="Q61" s="27"/>
+      <c r="R61" s="27"/>
+      <c r="S61" s="27"/>
+      <c r="T61" s="27"/>
+      <c r="U61" s="27"/>
+      <c r="V61" s="27"/>
+      <c r="W61" s="27"/>
+      <c r="X61" s="27"/>
+      <c r="Y61" s="27"/>
+      <c r="Z61" s="27"/>
+    </row>
+    <row r="62" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B61" s="6"/>
-      <c r="C61" s="50"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6"/>
-      <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="6"/>
-      <c r="I61" s="6"/>
-      <c r="J61" s="6"/>
-      <c r="K61" s="6"/>
-      <c r="L61" s="6"/>
-      <c r="M61" s="6"/>
-      <c r="N61" s="6"/>
-      <c r="O61" s="6"/>
-      <c r="P61" s="6"/>
-      <c r="Q61" s="6"/>
-      <c r="R61" s="6"/>
-      <c r="S61" s="6"/>
-      <c r="T61" s="6"/>
-      <c r="U61" s="6"/>
-      <c r="V61" s="6"/>
-      <c r="W61" s="6"/>
-      <c r="X61" s="6"/>
-      <c r="Y61" s="6"/>
-      <c r="Z61" s="6"/>
-    </row>
-    <row r="62" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="50"/>
       <c r="D62" s="6"/>
@@ -9472,7 +9479,7 @@
       <c r="Y249" s="6"/>
       <c r="Z249" s="6"/>
     </row>
-    <row r="250" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="6"/>
       <c r="B250" s="6"/>
       <c r="C250" s="50"/>
@@ -31172,6 +31179,34 @@
       <c r="Y1024" s="6"/>
       <c r="Z1024" s="6"/>
     </row>
+    <row r="1025" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1025" s="6"/>
+      <c r="B1025" s="6"/>
+      <c r="C1025" s="50"/>
+      <c r="D1025" s="6"/>
+      <c r="E1025" s="6"/>
+      <c r="F1025" s="6"/>
+      <c r="G1025" s="6"/>
+      <c r="H1025" s="6"/>
+      <c r="I1025" s="6"/>
+      <c r="J1025" s="6"/>
+      <c r="K1025" s="6"/>
+      <c r="L1025" s="6"/>
+      <c r="M1025" s="6"/>
+      <c r="N1025" s="6"/>
+      <c r="O1025" s="6"/>
+      <c r="P1025" s="6"/>
+      <c r="Q1025" s="6"/>
+      <c r="R1025" s="6"/>
+      <c r="S1025" s="6"/>
+      <c r="T1025" s="6"/>
+      <c r="U1025" s="6"/>
+      <c r="V1025" s="6"/>
+      <c r="W1025" s="6"/>
+      <c r="X1025" s="6"/>
+      <c r="Y1025" s="6"/>
+      <c r="Z1025" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -31186,7 +31221,7 @@
   <dimension ref="A1:Z949"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -31202,7 +31237,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>1</v>
@@ -31267,10 +31302,10 @@
         <v>49</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -31304,7 +31339,7 @@
         <v>153</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
@@ -31335,10 +31370,10 @@
         <v>49</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
@@ -31422,13 +31457,13 @@
     </row>
     <row r="8" spans="1:26" s="15" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>93</v>
-      </c>
       <c r="C8" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
@@ -57830,19 +57865,19 @@
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>77</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>78</v>
       </c>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
@@ -57857,19 +57892,19 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" s="19">
         <v>43900</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>

</xml_diff>

<commit_message>
refactor: remove file number restrictions
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/enroll.xlsx
+++ b/config/itech-aurum/forms/app/enroll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC81644-87E1-1E4C-B8A8-F2228DA9A5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478EBC0D-9ADD-5945-A511-62207CD13EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="170">
   <si>
     <t>type</t>
   </si>
@@ -530,9 +530,6 @@
   </si>
   <si>
     <t>data</t>
-  </si>
-  <si>
-    <t>regex(., '^[\w-]{5,9}$')</t>
   </si>
   <si>
     <t>Must be 5 – 9 alpha-numeric characters, cannot have white spaces</t>
@@ -2508,7 +2505,7 @@
   <dimension ref="A1:Z1028"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3915,11 +3912,9 @@
       <c r="F39" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="G39" s="48" t="s">
+      <c r="G39" s="48"/>
+      <c r="H39" s="38" t="s">
         <v>169</v>
-      </c>
-      <c r="H39" s="38" t="s">
-        <v>170</v>
       </c>
       <c r="I39" s="37"/>
       <c r="J39" s="37"/>

</xml_diff>

<commit_message>
feat: hidden WA option in enroll form
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/enroll.xlsx
+++ b/config/itech-aurum/forms/app/enroll.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53BD3CF-F068-8145-8BF8-A95CFA76A087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5B7346-2D17-DF45-8079-C9BDB09F3093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-1960" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="191">
   <si>
     <t>form_title</t>
   </si>
@@ -477,9 +477,6 @@
   </si>
   <si>
     <t>How would you like to receive follow up messages?</t>
-  </si>
-  <si>
-    <t>selected(${language_preference}, 'afrikaans') or selected(${language_preference}, 'zulu') or selected(${language_preference}, 'english')</t>
   </si>
   <si>
     <t>select_one same_sms_whatsapp_number</t>
@@ -1847,8 +1844,8 @@
   </sheetPr>
   <dimension ref="A1:Z1034"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3574,7 +3571,7 @@
     </row>
     <row r="48" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="35" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B48" s="35" t="s">
         <v>135</v>
@@ -3591,7 +3588,7 @@
         <v>137</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I48" s="31" t="s">
         <v>139</v>
@@ -3616,7 +3613,7 @@
     </row>
     <row r="49" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="35" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B49" s="35" t="s">
         <v>140</v>
@@ -3633,7 +3630,7 @@
         <v>137</v>
       </c>
       <c r="H49" s="30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I49" s="31" t="s">
         <v>139</v>
@@ -3702,15 +3699,17 @@
       <c r="C51" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="D51" s="31" t="s">
-        <v>147</v>
+      <c r="D51" s="31"/>
+      <c r="E51" s="30" t="s">
+        <v>55</v>
       </c>
-      <c r="E51" s="30"/>
       <c r="F51" s="90"/>
       <c r="G51" s="90"/>
       <c r="H51" s="90"/>
       <c r="I51" s="91"/>
-      <c r="J51" s="30"/>
+      <c r="J51" s="30" t="s">
+        <v>32</v>
+      </c>
       <c r="K51" s="30"/>
       <c r="L51" s="30"/>
       <c r="M51" s="30"/>
@@ -3730,18 +3729,20 @@
     </row>
     <row r="52" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="70" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B52" s="35" t="s">
         <v>34</v>
       </c>
       <c r="C52" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="D52" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="D52" s="31" t="s">
-        <v>150</v>
+      <c r="E52" s="30" t="s">
+        <v>55</v>
       </c>
-      <c r="E52" s="30"/>
       <c r="F52" s="90"/>
       <c r="G52" s="90"/>
       <c r="H52" s="90"/>
@@ -3769,15 +3770,17 @@
         <v>52</v>
       </c>
       <c r="B53" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="C53" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="C53" s="36" t="s">
+      <c r="D53" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="D53" s="31" t="s">
-        <v>153</v>
+      <c r="E53" s="30" t="s">
+        <v>55</v>
       </c>
-      <c r="E53" s="30"/>
       <c r="F53" s="90"/>
       <c r="G53" s="30" t="s">
         <v>137</v>
@@ -3809,10 +3812,10 @@
         <v>52</v>
       </c>
       <c r="B54" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C54" s="36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D54" s="31"/>
       <c r="E54" s="30"/>
@@ -3823,10 +3826,10 @@
         <v>112</v>
       </c>
       <c r="H54" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I54" s="30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J54" s="30"/>
       <c r="K54" s="30"/>
@@ -3909,14 +3912,14 @@
         <v>47</v>
       </c>
       <c r="B57" s="92" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C57" s="93" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D57" s="107"/>
       <c r="E57" s="98" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F57" s="99"/>
       <c r="G57" s="99"/>
@@ -3944,17 +3947,17 @@
     </row>
     <row r="58" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="103" t="s">
+        <v>160</v>
+      </c>
+      <c r="B58" s="94" t="s">
         <v>161</v>
       </c>
-      <c r="B58" s="94" t="s">
+      <c r="C58" s="95" t="s">
         <v>162</v>
-      </c>
-      <c r="C58" s="95" t="s">
-        <v>163</v>
       </c>
       <c r="D58" s="108"/>
       <c r="E58" s="100" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F58" s="99"/>
       <c r="G58" s="99"/>
@@ -3980,13 +3983,13 @@
     </row>
     <row r="59" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B59" s="94" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C59" s="95" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D59" s="108"/>
       <c r="E59" s="101"/>
@@ -4014,17 +4017,17 @@
     </row>
     <row r="60" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B60" s="94" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C60" s="95" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D60" s="108"/>
       <c r="E60" s="100" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F60" s="99"/>
       <c r="G60" s="99"/>
@@ -4050,13 +4053,13 @@
     </row>
     <row r="61" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B61" s="94" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C61" s="95" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D61" s="108"/>
       <c r="E61" s="101"/>
@@ -4084,13 +4087,13 @@
     </row>
     <row r="62" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B62" s="94" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C62" s="95" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D62" s="108"/>
       <c r="E62" s="101"/>
@@ -4118,13 +4121,13 @@
     </row>
     <row r="63" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B63" s="94" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C63" s="95" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D63" s="108"/>
       <c r="E63" s="101"/>
@@ -4152,13 +4155,13 @@
     </row>
     <row r="64" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B64" s="94" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C64" s="95" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D64" s="108"/>
       <c r="E64" s="101"/>
@@ -4186,13 +4189,13 @@
     </row>
     <row r="65" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B65" s="94" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C65" s="95" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D65" s="108"/>
       <c r="E65" s="101"/>
@@ -4220,13 +4223,13 @@
     </row>
     <row r="66" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B66" s="94" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C66" s="95" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D66" s="108"/>
       <c r="E66" s="101"/>
@@ -4254,13 +4257,13 @@
     </row>
     <row r="67" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B67" s="94" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C67" s="95" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D67" s="108"/>
       <c r="E67" s="101"/>
@@ -4288,13 +4291,13 @@
     </row>
     <row r="68" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B68" s="94" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C68" s="95" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D68" s="108"/>
       <c r="E68" s="101"/>
@@ -4322,13 +4325,13 @@
     </row>
     <row r="69" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B69" s="94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C69" s="95" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D69" s="108"/>
       <c r="E69" s="101"/>
@@ -4356,13 +4359,13 @@
     </row>
     <row r="70" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="104" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B70" s="96" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C70" s="97" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D70" s="109"/>
       <c r="E70" s="102"/>

</xml_diff>